<commit_message>
Making changes to plot excel sheet
</commit_message>
<xml_diff>
--- a/plots-data.xlsx
+++ b/plots-data.xlsx
@@ -1296,11 +1296,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="681139672"/>
-        <c:axId val="2983432"/>
+        <c:axId val="551250808"/>
+        <c:axId val="588489000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="681139672"/>
+        <c:axId val="551250808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1322,7 +1322,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1336,7 +1335,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2983432"/>
+        <c:crossAx val="588489000"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1344,7 +1343,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2983432"/>
+        <c:axId val="588489000"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -1379,7 +1378,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
@@ -1393,7 +1391,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="681139672"/>
+        <c:crossAx val="551250808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="4.0"/>
@@ -1401,7 +1399,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1851,11 +1848,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="513394216"/>
-        <c:axId val="529401880"/>
+        <c:axId val="551199864"/>
+        <c:axId val="551188152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="513394216"/>
+        <c:axId val="551199864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1900,7 +1897,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="529401880"/>
+        <c:crossAx val="551188152"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1908,7 +1905,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="529401880"/>
+        <c:axId val="551188152"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -1961,7 +1958,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="513394216"/>
+        <c:crossAx val="551199864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="4.0"/>
@@ -2428,11 +2425,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="476796488"/>
-        <c:axId val="529321832"/>
+        <c:axId val="551312168"/>
+        <c:axId val="551319768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="476796488"/>
+        <c:axId val="551312168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2477,7 +2474,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="529321832"/>
+        <c:crossAx val="551319768"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2485,7 +2482,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="529321832"/>
+        <c:axId val="551319768"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -2543,7 +2540,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="476796488"/>
+        <c:crossAx val="551312168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="4.0"/>
@@ -3010,11 +3007,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="742875704"/>
-        <c:axId val="526557512"/>
+        <c:axId val="551380376"/>
+        <c:axId val="551387976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="742875704"/>
+        <c:axId val="551380376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3060,7 +3057,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="526557512"/>
+        <c:crossAx val="551387976"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3068,7 +3065,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="526557512"/>
+        <c:axId val="551387976"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -3127,7 +3124,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="742875704"/>
+        <c:crossAx val="551380376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="4.0"/>
@@ -3832,11 +3829,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="513420472"/>
-        <c:axId val="528817816"/>
+        <c:axId val="551447848"/>
+        <c:axId val="551453752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="513420472"/>
+        <c:axId val="551447848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3863,6 +3860,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -3886,7 +3884,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="528817816"/>
+        <c:crossAx val="551453752"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3894,7 +3892,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="528817816"/>
+        <c:axId val="551453752"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -3924,6 +3922,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
@@ -3947,7 +3946,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="513420472"/>
+        <c:crossAx val="551447848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="4.0"/>
@@ -3956,6 +3955,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -4998,11 +4998,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="414960744"/>
-        <c:axId val="527051048"/>
+        <c:axId val="551533144"/>
+        <c:axId val="597692440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="414960744"/>
+        <c:axId val="551533144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5048,7 +5048,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="527051048"/>
+        <c:crossAx val="597692440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5056,7 +5056,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="527051048"/>
+        <c:axId val="597692440"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -5110,7 +5110,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="414960744"/>
+        <c:crossAx val="551533144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5597,11 +5597,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="720925656"/>
-        <c:axId val="513398360"/>
+        <c:axId val="597728904"/>
+        <c:axId val="597735016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="720925656"/>
+        <c:axId val="597728904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5651,7 +5651,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="513398360"/>
+        <c:crossAx val="597735016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5659,7 +5659,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="513398360"/>
+        <c:axId val="597735016"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -5712,7 +5712,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="720925656"/>
+        <c:crossAx val="597728904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5764,7 +5764,17 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.224378284293411"/>
+          <c:y val="0.154993813958395"/>
+          <c:w val="0.733516452548695"/>
+          <c:h val="0.722472690304699"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -6194,11 +6204,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="721337448"/>
-        <c:axId val="743014968"/>
+        <c:axId val="597779656"/>
+        <c:axId val="597787448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="721337448"/>
+        <c:axId val="597779656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6244,7 +6254,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="743014968"/>
+        <c:crossAx val="597787448"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6252,7 +6262,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="743014968"/>
+        <c:axId val="597787448"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -6311,10 +6321,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="721337448"/>
+        <c:crossAx val="597779656"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-        <c:majorUnit val="4.0"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -6350,7 +6359,17 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.127640862078219"/>
+          <c:y val="0.128623629719854"/>
+          <c:w val="0.639075819027977"/>
+          <c:h val="0.716382556321751"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -6770,11 +6789,11 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln>
+            <a:ln w="76200" cmpd="sng">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:prstDash val="sysDash"/>
+              <a:prstDash val="dash"/>
             </a:ln>
           </c:spPr>
           <c:marker>
@@ -6846,11 +6865,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="526769240"/>
-        <c:axId val="512902376"/>
+        <c:axId val="597836616"/>
+        <c:axId val="597842728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="526769240"/>
+        <c:axId val="597836616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6901,7 +6920,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="512902376"/>
+        <c:crossAx val="597842728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6909,7 +6928,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="512902376"/>
+        <c:axId val="597842728"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -6963,9 +6982,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="526769240"/>
+        <c:crossAx val="597836616"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -7016,7 +7035,17 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.252649242082625"/>
+          <c:y val="0.178825354498419"/>
+          <c:w val="0.730830934128829"/>
+          <c:h val="0.65374137338264"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -7560,92 +7589,6 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1160.27</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="8"/>
-          <c:order val="7"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>data!$A$40</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>keller4</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="57150" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="3366FF"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:spPr>
-              <a:ln w="57150" cmpd="sng">
-                <a:solidFill>
-                  <a:srgbClr val="3366FF"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>data!$F$1:$K$1</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>data!$B$40:$G$40</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0" formatCode="0.00">
-                  <c:v>23.3548</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.4564</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.68531</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.9381</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.57895</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.53022</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7662,11 +7605,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="528620936"/>
-        <c:axId val="513521752"/>
+        <c:axId val="597900392"/>
+        <c:axId val="597908104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="528620936"/>
+        <c:axId val="597900392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7717,7 +7660,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="513521752"/>
+        <c:crossAx val="597908104"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7725,7 +7668,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="513521752"/>
+        <c:axId val="597908104"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -7779,10 +7722,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="528620936"/>
+        <c:crossAx val="597900392"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-        <c:majorUnit val="4.0"/>
+        <c:crossBetween val="midCat"/>
         <c:minorUnit val="4.0"/>
       </c:valAx>
     </c:plotArea>
@@ -7827,10 +7769,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.170596506969045"/>
-          <c:y val="0.0693266832917706"/>
-          <c:w val="0.601505654131151"/>
-          <c:h val="0.808167180474012"/>
+          <c:x val="0.169614188697926"/>
+          <c:y val="0.171299696476488"/>
+          <c:w val="0.592297530488247"/>
+          <c:h val="0.678796199357762"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -8397,94 +8339,8 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="8"/>
+          <c:idx val="0"/>
           <c:order val="7"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>data!$A$40</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>keller4</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="57150" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="3366FF"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:spPr>
-              <a:ln w="57150" cmpd="sng">
-                <a:solidFill>
-                  <a:srgbClr val="3366FF"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>data!$L$1:$Q$1</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>data!$H$40:$M$40</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0" formatCode="0.0000">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.038581055130756</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.107920236539432</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.948946598141656</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14.79134868108553</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>15.26238057272811</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="8"/>
           <c:tx>
             <c:strRef>
               <c:f>data!$A$41</c:f>
@@ -8497,11 +8353,11 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln>
+            <a:ln w="76200" cmpd="sng">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:prstDash val="sysDash"/>
+              <a:prstDash val="dash"/>
             </a:ln>
           </c:spPr>
           <c:marker>
@@ -8509,7 +8365,6 @@
           </c:marker>
           <c:dPt>
             <c:idx val="4"/>
-            <c:marker/>
             <c:bubble3D val="0"/>
           </c:dPt>
           <c:cat>
@@ -8578,11 +8433,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="456460952"/>
-        <c:axId val="720762904"/>
+        <c:axId val="597971144"/>
+        <c:axId val="597976840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="456460952"/>
+        <c:axId val="597971144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8628,7 +8483,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="720762904"/>
+        <c:crossAx val="597976840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8636,7 +8491,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="720762904"/>
+        <c:axId val="597976840"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -8690,14 +8545,23 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="456460952"/>
+        <c:crossAx val="597971144"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.78689570916895"/>
+          <c:y val="0.276264339532989"/>
+          <c:w val="0.211689587426326"/>
+          <c:h val="0.495794271203464"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -9157,11 +9021,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2691688"/>
-        <c:axId val="3010712"/>
+        <c:axId val="588543976"/>
+        <c:axId val="588551784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2691688"/>
+        <c:axId val="588543976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9188,7 +9052,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -9202,7 +9065,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="3010712"/>
+        <c:crossAx val="588551784"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9210,7 +9073,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="3010712"/>
+        <c:axId val="588551784"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -9245,7 +9108,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
@@ -9259,7 +9121,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2691688"/>
+        <c:crossAx val="588543976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="4.0"/>
@@ -9267,7 +9129,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -9957,11 +9818,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="456497768"/>
-        <c:axId val="456500776"/>
+        <c:axId val="598048712"/>
+        <c:axId val="598051720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="456497768"/>
+        <c:axId val="598048712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9971,7 +9832,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="456500776"/>
+        <c:crossAx val="598051720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9979,7 +9840,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="456500776"/>
+        <c:axId val="598051720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9990,14 +9851,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="456497768"/>
+        <c:crossAx val="598048712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -10362,11 +10222,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="513310664"/>
-        <c:axId val="527301400"/>
+        <c:axId val="598086056"/>
+        <c:axId val="598089176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="513310664"/>
+        <c:axId val="598086056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10376,7 +10236,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="527301400"/>
+        <c:crossAx val="598089176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10384,7 +10244,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="527301400"/>
+        <c:axId val="598089176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10395,14 +10255,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="513310664"/>
+        <c:crossAx val="598086056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -10767,11 +10626,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="512822584"/>
-        <c:axId val="526920296"/>
+        <c:axId val="598127416"/>
+        <c:axId val="598130536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="512822584"/>
+        <c:axId val="598127416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10781,7 +10640,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="526920296"/>
+        <c:crossAx val="598130536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10789,7 +10648,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="526920296"/>
+        <c:axId val="598130536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10800,14 +10659,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="512822584"/>
+        <c:crossAx val="598127416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -11172,11 +11030,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="742506744"/>
-        <c:axId val="512954104"/>
+        <c:axId val="598168904"/>
+        <c:axId val="598172024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="742506744"/>
+        <c:axId val="598168904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11186,7 +11044,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="512954104"/>
+        <c:crossAx val="598172024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11194,7 +11052,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="512954104"/>
+        <c:axId val="598172024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11205,14 +11063,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="742506744"/>
+        <c:crossAx val="598168904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -11657,11 +11514,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2761656"/>
-        <c:axId val="2548024"/>
+        <c:axId val="588594568"/>
+        <c:axId val="588602136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2761656"/>
+        <c:axId val="588594568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11683,7 +11540,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -11697,7 +11553,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2548024"/>
+        <c:crossAx val="588602136"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11705,7 +11561,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2548024"/>
+        <c:axId val="588602136"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -11735,7 +11591,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
@@ -11749,7 +11604,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2761656"/>
+        <c:crossAx val="588594568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="4.0"/>
@@ -11757,7 +11612,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -12207,11 +12061,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="456219368"/>
-        <c:axId val="742822456"/>
+        <c:axId val="588645784"/>
+        <c:axId val="588653352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="456219368"/>
+        <c:axId val="588645784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12233,7 +12087,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -12247,7 +12100,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="742822456"/>
+        <c:crossAx val="588653352"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12255,7 +12108,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="742822456"/>
+        <c:axId val="588653352"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -12290,7 +12143,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
@@ -12304,7 +12156,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="456219368"/>
+        <c:crossAx val="588645784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="4.0"/>
@@ -12312,7 +12164,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -12782,11 +12633,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="743096920"/>
-        <c:axId val="529150088"/>
+        <c:axId val="588693480"/>
+        <c:axId val="588696680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="743096920"/>
+        <c:axId val="588693480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12796,7 +12647,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="529150088"/>
+        <c:crossAx val="588696680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12804,7 +12655,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="529150088"/>
+        <c:axId val="588696680"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -12816,14 +12667,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="743096920"/>
+        <c:crossAx val="588693480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -13498,11 +13348,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="481373240"/>
-        <c:axId val="527162360"/>
+        <c:axId val="588753560"/>
+        <c:axId val="588756568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="481373240"/>
+        <c:axId val="588753560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13512,7 +13362,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="527162360"/>
+        <c:crossAx val="588756568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13520,7 +13370,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="527162360"/>
+        <c:axId val="588756568"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -13532,14 +13382,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="481373240"/>
+        <c:crossAx val="588753560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -14214,11 +14063,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="526635448"/>
-        <c:axId val="456347800"/>
+        <c:axId val="588809432"/>
+        <c:axId val="588812440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="526635448"/>
+        <c:axId val="588809432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14228,7 +14077,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="456347800"/>
+        <c:crossAx val="588812440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14236,7 +14085,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="456347800"/>
+        <c:axId val="588812440"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -14248,14 +14097,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="526635448"/>
+        <c:crossAx val="588809432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -15108,11 +14956,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="526737080"/>
-        <c:axId val="513667784"/>
+        <c:axId val="48805976"/>
+        <c:axId val="48813256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="526737080"/>
+        <c:axId val="48805976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15157,7 +15005,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="513667784"/>
+        <c:crossAx val="48813256"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15165,7 +15013,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="513667784"/>
+        <c:axId val="48813256"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -15223,7 +15071,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="526737080"/>
+        <c:crossAx val="48805976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="4.0"/>
@@ -15690,11 +15538,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="720980024"/>
-        <c:axId val="742641784"/>
+        <c:axId val="48848600"/>
+        <c:axId val="48856440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="720980024"/>
+        <c:axId val="48848600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15744,7 +15592,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="742641784"/>
+        <c:crossAx val="48856440"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15752,7 +15600,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="742641784"/>
+        <c:axId val="48856440"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -15810,7 +15658,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="720980024"/>
+        <c:crossAx val="48848600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="4.0"/>
@@ -16399,8 +16247,8 @@
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>800100</xdr:colOff>
-      <xdr:row>263</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:row>276</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16423,16 +16271,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>218</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>214</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>271</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>276</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -19067,7 +18915,6 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -19101,8 +18948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="I185" workbookViewId="0">
-      <selection activeCell="Q211" sqref="Q211"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="M142" sqref="M142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
half-completed changes for new community extraction algo
</commit_message>
<xml_diff>
--- a/plots-data.xlsx
+++ b/plots-data.xlsx
@@ -4,13 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20480" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="180" yWindow="340" windowWidth="32980" windowHeight="17540" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="plots" sheetId="2" r:id="rId2"/>
     <sheet name="plots_goodonly" sheetId="4" r:id="rId3"/>
     <sheet name="data_12" sheetId="3" r:id="rId4"/>
+    <sheet name="data_communities_WRONG!" sheetId="5" r:id="rId5"/>
+    <sheet name="data_comm_correct" sheetId="6" r:id="rId6"/>
+    <sheet name="data_comm_paper" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="out_12x" localSheetId="3">data_12!#REF!</definedName>
@@ -53,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="71">
   <si>
     <t>brock200_2</t>
   </si>
@@ -156,13 +159,125 @@
   <si>
     <t>Ideal</t>
   </si>
+  <si>
+    <t>Graph:</t>
+  </si>
+  <si>
+    <t>N=1000</t>
+  </si>
+  <si>
+    <t>k=10</t>
+  </si>
+  <si>
+    <t>maxk=50</t>
+  </si>
+  <si>
+    <t>mu=0.1</t>
+  </si>
+  <si>
+    <t>t1=2</t>
+  </si>
+  <si>
+    <t>t2=1</t>
+  </si>
+  <si>
+    <t>minc=20</t>
+  </si>
+  <si>
+    <t>maxc=50</t>
+  </si>
+  <si>
+    <t>on=100</t>
+  </si>
+  <si>
+    <t>om=2</t>
+  </si>
+  <si>
+    <t>Ground Truth</t>
+  </si>
+  <si>
+    <t>Num Comms</t>
+  </si>
+  <si>
+    <t>NumComms</t>
+  </si>
+  <si>
+    <t>Omega</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>Cfinder (k=?)</t>
+  </si>
+  <si>
+    <t>we consider only the bext k value for cfinder</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>mu</t>
+  </si>
+  <si>
+    <t>On</t>
+  </si>
+  <si>
+    <t>Om</t>
+  </si>
+  <si>
+    <t>OurAlgo(c=10)</t>
+  </si>
+  <si>
+    <t>OurAlgo(c=0)</t>
+  </si>
+  <si>
+    <t>OurAlgo(c=20)</t>
+  </si>
+  <si>
+    <t>OurAlgo(c=30)</t>
+  </si>
+  <si>
+    <t>type=LFR</t>
+  </si>
+  <si>
+    <t>Best k</t>
+  </si>
+  <si>
+    <t>Shared Nodes</t>
+  </si>
+  <si>
+    <t>best k</t>
+  </si>
+  <si>
+    <t>OurAlgo(c=5)</t>
+  </si>
+  <si>
+    <t>OurAlgo(c=2)</t>
+  </si>
+  <si>
+    <t>C5%Cfinder</t>
+  </si>
+  <si>
+    <t>C2%Cfinder</t>
+  </si>
+  <si>
+    <t>C0%Cfinder</t>
+  </si>
+  <si>
+    <t>Speedup</t>
+  </si>
+  <si>
+    <t>&amp;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -250,7 +365,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="87">
+  <cellStyleXfs count="191">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -338,8 +453,112 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -363,8 +582,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="87">
+  <cellStyles count="191">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -408,6 +631,58 @@
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -451,6 +726,58 @@
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1296,11 +1623,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="551250808"/>
-        <c:axId val="588489000"/>
+        <c:axId val="2115907672"/>
+        <c:axId val="2089831752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="551250808"/>
+        <c:axId val="2115907672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1335,7 +1662,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="588489000"/>
+        <c:crossAx val="2089831752"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1343,7 +1670,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="588489000"/>
+        <c:axId val="2089831752"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -1391,7 +1718,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="551250808"/>
+        <c:crossAx val="2115907672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="4.0"/>
@@ -1848,11 +2175,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="551199864"/>
-        <c:axId val="551188152"/>
+        <c:axId val="2113946584"/>
+        <c:axId val="2113939000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="551199864"/>
+        <c:axId val="2113946584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1897,7 +2224,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="551188152"/>
+        <c:crossAx val="2113939000"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1905,7 +2232,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="551188152"/>
+        <c:axId val="2113939000"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -1958,7 +2285,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="551199864"/>
+        <c:crossAx val="2113946584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="4.0"/>
@@ -2425,11 +2752,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="551312168"/>
-        <c:axId val="551319768"/>
+        <c:axId val="2118181432"/>
+        <c:axId val="2118189032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="551312168"/>
+        <c:axId val="2118181432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2474,7 +2801,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="551319768"/>
+        <c:crossAx val="2118189032"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2482,7 +2809,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="551319768"/>
+        <c:axId val="2118189032"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -2540,7 +2867,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="551312168"/>
+        <c:crossAx val="2118181432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="4.0"/>
@@ -3007,11 +3334,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="551380376"/>
-        <c:axId val="551387976"/>
+        <c:axId val="2118249432"/>
+        <c:axId val="2118257032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="551380376"/>
+        <c:axId val="2118249432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3033,7 +3360,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -3057,7 +3383,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="551387976"/>
+        <c:crossAx val="2118257032"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3065,7 +3391,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="551387976"/>
+        <c:axId val="2118257032"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -3100,7 +3426,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
@@ -3124,7 +3449,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="551380376"/>
+        <c:crossAx val="2118249432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="4.0"/>
@@ -3132,7 +3457,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -3829,11 +4153,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="551447848"/>
-        <c:axId val="551453752"/>
+        <c:axId val="2118317448"/>
+        <c:axId val="2118323352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="551447848"/>
+        <c:axId val="2118317448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3860,7 +4184,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -3884,7 +4207,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="551453752"/>
+        <c:crossAx val="2118323352"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3892,7 +4215,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="551453752"/>
+        <c:axId val="2118323352"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -3922,7 +4245,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
@@ -3946,7 +4268,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="551447848"/>
+        <c:crossAx val="2118317448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="4.0"/>
@@ -3955,7 +4277,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -4998,11 +5319,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="551533144"/>
-        <c:axId val="597692440"/>
+        <c:axId val="2118402600"/>
+        <c:axId val="2118408296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="551533144"/>
+        <c:axId val="2118402600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5024,7 +5345,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -5048,7 +5368,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="597692440"/>
+        <c:crossAx val="2118408296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5056,7 +5376,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="597692440"/>
+        <c:axId val="2118408296"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -5086,7 +5406,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="0"/>
@@ -5110,14 +5429,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="551533144"/>
+        <c:crossAx val="2118402600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -5597,11 +5915,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="597728904"/>
-        <c:axId val="597735016"/>
+        <c:axId val="2118444408"/>
+        <c:axId val="2118450520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="597728904"/>
+        <c:axId val="2118444408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5651,7 +5969,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="597735016"/>
+        <c:crossAx val="2118450520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5659,7 +5977,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="597735016"/>
+        <c:axId val="2118450520"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -5712,7 +6030,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="597728904"/>
+        <c:crossAx val="2118444408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6204,11 +6522,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="597779656"/>
-        <c:axId val="597787448"/>
+        <c:axId val="2117285880"/>
+        <c:axId val="2117293672"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="597779656"/>
+        <c:axId val="2117285880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6230,7 +6548,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -6254,7 +6571,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="597787448"/>
+        <c:crossAx val="2117293672"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6262,7 +6579,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="597787448"/>
+        <c:axId val="2117293672"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -6297,7 +6614,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="0"/>
@@ -6321,7 +6637,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="597779656"/>
+        <c:crossAx val="2117285880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6865,11 +7181,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="597836616"/>
-        <c:axId val="597842728"/>
+        <c:axId val="2117346264"/>
+        <c:axId val="2117352360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="597836616"/>
+        <c:axId val="2117346264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6896,7 +7212,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -6920,7 +7235,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="597842728"/>
+        <c:crossAx val="2117352360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6928,7 +7243,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="597842728"/>
+        <c:axId val="2117352360"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -6958,7 +7273,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -6982,14 +7296,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="597836616"/>
+        <c:crossAx val="2117346264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -7605,11 +7918,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="597900392"/>
-        <c:axId val="597908104"/>
+        <c:axId val="2071831384"/>
+        <c:axId val="2071836952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="597900392"/>
+        <c:axId val="2071831384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7636,7 +7949,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -7660,7 +7972,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="597908104"/>
+        <c:crossAx val="2071836952"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7668,7 +7980,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="597908104"/>
+        <c:axId val="2071836952"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -7698,7 +8010,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
@@ -7722,7 +8033,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="597900392"/>
+        <c:crossAx val="2071831384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="4.0"/>
@@ -8433,11 +8744,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="597971144"/>
-        <c:axId val="597976840"/>
+        <c:axId val="2117361368"/>
+        <c:axId val="2117304744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="597971144"/>
+        <c:axId val="2117361368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8459,7 +8770,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -8483,7 +8793,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="597976840"/>
+        <c:crossAx val="2117304744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8491,7 +8801,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="597976840"/>
+        <c:axId val="2117304744"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -8521,7 +8831,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="0"/>
@@ -8545,7 +8854,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="597971144"/>
+        <c:crossAx val="2117361368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9021,11 +9330,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="588543976"/>
-        <c:axId val="588551784"/>
+        <c:axId val="2115981720"/>
+        <c:axId val="2115989528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="588543976"/>
+        <c:axId val="2115981720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9065,7 +9374,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="588551784"/>
+        <c:crossAx val="2115989528"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9073,7 +9382,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="588551784"/>
+        <c:axId val="2115989528"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -9121,7 +9430,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="588543976"/>
+        <c:crossAx val="2115981720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="4.0"/>
@@ -9818,11 +10127,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="598048712"/>
-        <c:axId val="598051720"/>
+        <c:axId val="2117477880"/>
+        <c:axId val="2117480888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="598048712"/>
+        <c:axId val="2117477880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9832,7 +10141,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="598051720"/>
+        <c:crossAx val="2117480888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9840,7 +10149,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="598051720"/>
+        <c:axId val="2117480888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9851,7 +10160,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="598048712"/>
+        <c:crossAx val="2117477880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10222,11 +10531,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="598086056"/>
-        <c:axId val="598089176"/>
+        <c:axId val="2117515176"/>
+        <c:axId val="2117518296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="598086056"/>
+        <c:axId val="2117515176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10236,7 +10545,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="598089176"/>
+        <c:crossAx val="2117518296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10244,7 +10553,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="598089176"/>
+        <c:axId val="2117518296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10255,7 +10564,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="598086056"/>
+        <c:crossAx val="2117515176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10626,11 +10935,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="598127416"/>
-        <c:axId val="598130536"/>
+        <c:axId val="2117556536"/>
+        <c:axId val="2117559656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="598127416"/>
+        <c:axId val="2117556536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10640,7 +10949,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="598130536"/>
+        <c:crossAx val="2117559656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10648,7 +10957,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="598130536"/>
+        <c:axId val="2117559656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10659,7 +10968,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="598127416"/>
+        <c:crossAx val="2117556536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11030,11 +11339,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="598168904"/>
-        <c:axId val="598172024"/>
+        <c:axId val="2117598024"/>
+        <c:axId val="2117601144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="598168904"/>
+        <c:axId val="2117598024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11044,7 +11353,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="598172024"/>
+        <c:crossAx val="2117601144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11052,7 +11361,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="598172024"/>
+        <c:axId val="2117601144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11063,7 +11372,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="598168904"/>
+        <c:crossAx val="2117598024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11514,11 +11823,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="588594568"/>
-        <c:axId val="588602136"/>
+        <c:axId val="2117096728"/>
+        <c:axId val="2117104216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="588594568"/>
+        <c:axId val="2117096728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11553,7 +11862,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="588602136"/>
+        <c:crossAx val="2117104216"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11561,7 +11870,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="588602136"/>
+        <c:axId val="2117104216"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -11604,7 +11913,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="588594568"/>
+        <c:crossAx val="2117096728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="4.0"/>
@@ -12061,11 +12370,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="588645784"/>
-        <c:axId val="588653352"/>
+        <c:axId val="2117147608"/>
+        <c:axId val="2117155176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="588645784"/>
+        <c:axId val="2117147608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12100,7 +12409,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="588653352"/>
+        <c:crossAx val="2117155176"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12108,7 +12417,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="588653352"/>
+        <c:axId val="2117155176"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -12156,7 +12465,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="588645784"/>
+        <c:crossAx val="2117147608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="4.0"/>
@@ -12633,11 +12942,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="588693480"/>
-        <c:axId val="588696680"/>
+        <c:axId val="2117195304"/>
+        <c:axId val="2117198504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="588693480"/>
+        <c:axId val="2117195304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12647,7 +12956,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="588696680"/>
+        <c:crossAx val="2117198504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12655,7 +12964,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="588696680"/>
+        <c:axId val="2117198504"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -12667,7 +12976,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="588693480"/>
+        <c:crossAx val="2117195304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13348,11 +13657,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="588753560"/>
-        <c:axId val="588756568"/>
+        <c:axId val="2117255400"/>
+        <c:axId val="2117258408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="588753560"/>
+        <c:axId val="2117255400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13362,7 +13671,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="588756568"/>
+        <c:crossAx val="2117258408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13370,7 +13679,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="588756568"/>
+        <c:axId val="2117258408"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -13382,7 +13691,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="588753560"/>
+        <c:crossAx val="2117255400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14063,11 +14372,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="588809432"/>
-        <c:axId val="588812440"/>
+        <c:axId val="2116097512"/>
+        <c:axId val="2116100520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="588809432"/>
+        <c:axId val="2116097512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14077,7 +14386,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="588812440"/>
+        <c:crossAx val="2116100520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14085,7 +14394,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="588812440"/>
+        <c:axId val="2116100520"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -14097,7 +14406,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="588809432"/>
+        <c:crossAx val="2116097512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14956,11 +15265,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="48805976"/>
-        <c:axId val="48813256"/>
+        <c:axId val="2116192760"/>
+        <c:axId val="2116200040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="48805976"/>
+        <c:axId val="2116192760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15005,7 +15314,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48813256"/>
+        <c:crossAx val="2116200040"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15013,7 +15322,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="48813256"/>
+        <c:axId val="2116200040"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -15071,7 +15380,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48805976"/>
+        <c:crossAx val="2116192760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="4.0"/>
@@ -15538,11 +15847,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="48848600"/>
-        <c:axId val="48856440"/>
+        <c:axId val="2116235224"/>
+        <c:axId val="2116243064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="48848600"/>
+        <c:axId val="2116235224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15592,7 +15901,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48856440"/>
+        <c:crossAx val="2116243064"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15600,7 +15909,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="48856440"/>
+        <c:axId val="2116243064"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -15658,7 +15967,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48848600"/>
+        <c:crossAx val="2116235224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="4.0"/>
@@ -18948,7 +19257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A134" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="A134" workbookViewId="0">
       <selection activeCell="M142" sqref="M142"/>
     </sheetView>
   </sheetViews>
@@ -20465,4 +20774,3050 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:AD15"/>
+  <sheetViews>
+    <sheetView showRuler="0" topLeftCell="M1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="Q17" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:30">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" t="s">
+        <v>43</v>
+      </c>
+      <c r="L3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30">
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" t="s">
+        <v>50</v>
+      </c>
+      <c r="L6" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>56</v>
+      </c>
+      <c r="V6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" t="s">
+        <v>49</v>
+      </c>
+      <c r="J7" t="s">
+        <v>61</v>
+      </c>
+      <c r="K7" t="s">
+        <v>47</v>
+      </c>
+      <c r="L7" t="s">
+        <v>62</v>
+      </c>
+      <c r="M7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N7" t="s">
+        <v>49</v>
+      </c>
+      <c r="O7" t="s">
+        <v>63</v>
+      </c>
+      <c r="P7" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>62</v>
+      </c>
+      <c r="R7" t="s">
+        <v>48</v>
+      </c>
+      <c r="S7" t="s">
+        <v>49</v>
+      </c>
+      <c r="T7" t="s">
+        <v>63</v>
+      </c>
+      <c r="U7" t="s">
+        <v>47</v>
+      </c>
+      <c r="V7" t="s">
+        <v>62</v>
+      </c>
+      <c r="W7" t="s">
+        <v>48</v>
+      </c>
+      <c r="X7" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30">
+      <c r="A8">
+        <v>1000</v>
+      </c>
+      <c r="B8">
+        <v>0.1</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="E8">
+        <v>34</v>
+      </c>
+      <c r="F8">
+        <v>37</v>
+      </c>
+      <c r="G8">
+        <v>55</v>
+      </c>
+      <c r="H8">
+        <v>0.84220700000000004</v>
+      </c>
+      <c r="I8">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="J8">
+        <v>4</v>
+      </c>
+      <c r="K8">
+        <v>42</v>
+      </c>
+      <c r="L8">
+        <v>17</v>
+      </c>
+      <c r="M8">
+        <v>0.10109700000000001</v>
+      </c>
+      <c r="N8">
+        <v>2.78115E-3</v>
+      </c>
+      <c r="O8">
+        <v>4</v>
+      </c>
+      <c r="P8">
+        <v>42</v>
+      </c>
+      <c r="Q8">
+        <v>53</v>
+      </c>
+      <c r="R8">
+        <v>0.61462300000000003</v>
+      </c>
+      <c r="S8">
+        <v>0.118793</v>
+      </c>
+      <c r="T8">
+        <v>4</v>
+      </c>
+      <c r="U8">
+        <v>47</v>
+      </c>
+      <c r="V8">
+        <v>63</v>
+      </c>
+      <c r="W8">
+        <v>0.74676100000000001</v>
+      </c>
+      <c r="X8">
+        <v>0.40734999999999999</v>
+      </c>
+      <c r="Y8">
+        <v>4</v>
+      </c>
+      <c r="Z8">
+        <v>44</v>
+      </c>
+      <c r="AA8">
+        <v>63</v>
+      </c>
+      <c r="AB8">
+        <v>0.80199200000000004</v>
+      </c>
+      <c r="AC8">
+        <v>0.9375</v>
+      </c>
+      <c r="AD8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30">
+      <c r="A9">
+        <v>1000</v>
+      </c>
+      <c r="B9">
+        <v>0.1</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="E9">
+        <v>44</v>
+      </c>
+      <c r="F9">
+        <v>62</v>
+      </c>
+      <c r="G9">
+        <v>153</v>
+      </c>
+      <c r="H9">
+        <v>0.40223599999999998</v>
+      </c>
+      <c r="I9">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="J9">
+        <v>4</v>
+      </c>
+      <c r="K9">
+        <v>63</v>
+      </c>
+      <c r="L9">
+        <v>82</v>
+      </c>
+      <c r="M9">
+        <v>9.7805500000000004E-2</v>
+      </c>
+      <c r="N9">
+        <v>3.5758000000000001E-3</v>
+      </c>
+      <c r="O9">
+        <v>4</v>
+      </c>
+      <c r="P9">
+        <v>64</v>
+      </c>
+      <c r="Q9">
+        <v>147</v>
+      </c>
+      <c r="R9">
+        <v>0.32917800000000003</v>
+      </c>
+      <c r="S9">
+        <v>0.123428</v>
+      </c>
+      <c r="T9">
+        <v>4</v>
+      </c>
+      <c r="U9">
+        <v>64</v>
+      </c>
+      <c r="V9">
+        <v>152</v>
+      </c>
+      <c r="W9">
+        <v>0.37624000000000002</v>
+      </c>
+      <c r="X9">
+        <v>0.410576</v>
+      </c>
+      <c r="Y9">
+        <v>4</v>
+      </c>
+      <c r="Z9">
+        <v>66</v>
+      </c>
+      <c r="AA9">
+        <v>155</v>
+      </c>
+      <c r="AB9">
+        <v>0.392239</v>
+      </c>
+      <c r="AC9">
+        <v>0.866371</v>
+      </c>
+      <c r="AD9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30">
+      <c r="A10" s="16">
+        <v>1000</v>
+      </c>
+      <c r="B10" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="C10" s="16">
+        <v>8</v>
+      </c>
+      <c r="D10" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="E10" s="16">
+        <v>51</v>
+      </c>
+      <c r="F10" s="16">
+        <v>58</v>
+      </c>
+      <c r="G10" s="16">
+        <v>30</v>
+      </c>
+      <c r="H10">
+        <v>-1.98088E-3</v>
+      </c>
+      <c r="I10">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="J10">
+        <v>4</v>
+      </c>
+      <c r="K10">
+        <v>48</v>
+      </c>
+      <c r="L10">
+        <v>19</v>
+      </c>
+      <c r="M10">
+        <v>-4.5666000000000001E-4</v>
+      </c>
+      <c r="N10">
+        <v>3.1728699999999999E-3</v>
+      </c>
+      <c r="O10">
+        <v>4</v>
+      </c>
+      <c r="P10">
+        <v>64</v>
+      </c>
+      <c r="Q10">
+        <v>37</v>
+      </c>
+      <c r="R10">
+        <v>-9.2070800000000001E-4</v>
+      </c>
+      <c r="S10">
+        <v>0.168407</v>
+      </c>
+      <c r="T10">
+        <v>4</v>
+      </c>
+      <c r="U10">
+        <v>67</v>
+      </c>
+      <c r="V10">
+        <v>42</v>
+      </c>
+      <c r="W10">
+        <v>-2.3766099999999999E-3</v>
+      </c>
+      <c r="X10">
+        <v>0.56982100000000002</v>
+      </c>
+      <c r="Y10">
+        <v>4</v>
+      </c>
+      <c r="Z10">
+        <v>63</v>
+      </c>
+      <c r="AA10">
+        <v>38</v>
+      </c>
+      <c r="AB10">
+        <v>-2.18966E-3</v>
+      </c>
+      <c r="AC10">
+        <v>1.26108</v>
+      </c>
+      <c r="AD10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30">
+      <c r="A11" s="16">
+        <v>1000</v>
+      </c>
+      <c r="B11" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="C11" s="16">
+        <v>8</v>
+      </c>
+      <c r="D11" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="E11" s="16">
+        <v>130</v>
+      </c>
+      <c r="F11" s="16">
+        <v>74</v>
+      </c>
+      <c r="G11" s="16">
+        <v>68</v>
+      </c>
+      <c r="H11">
+        <v>0.03</v>
+      </c>
+      <c r="I11">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="J11">
+        <v>4</v>
+      </c>
+      <c r="K11">
+        <v>59</v>
+      </c>
+      <c r="L11">
+        <v>42</v>
+      </c>
+      <c r="M11">
+        <v>1.3283100000000001E-2</v>
+      </c>
+      <c r="N11">
+        <v>2.1381400000000002E-3</v>
+      </c>
+      <c r="O11">
+        <v>4</v>
+      </c>
+      <c r="P11">
+        <v>80</v>
+      </c>
+      <c r="Q11">
+        <v>75</v>
+      </c>
+      <c r="R11">
+        <v>2.9114999999999999E-2</v>
+      </c>
+      <c r="S11">
+        <v>3.5094E-2</v>
+      </c>
+      <c r="T11">
+        <v>4</v>
+      </c>
+      <c r="U11">
+        <v>76</v>
+      </c>
+      <c r="V11">
+        <v>68</v>
+      </c>
+      <c r="W11">
+        <v>3.1461599999999999E-2</v>
+      </c>
+      <c r="X11">
+        <v>0.101327</v>
+      </c>
+      <c r="Y11">
+        <v>4</v>
+      </c>
+      <c r="Z11">
+        <v>75</v>
+      </c>
+      <c r="AA11">
+        <v>70</v>
+      </c>
+      <c r="AB11">
+        <v>3.1435699999999997E-2</v>
+      </c>
+      <c r="AC11">
+        <v>0.20366699999999999</v>
+      </c>
+      <c r="AD11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30">
+      <c r="A12" s="16">
+        <v>1000</v>
+      </c>
+      <c r="B12" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="C12" s="16">
+        <v>2</v>
+      </c>
+      <c r="D12" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="E12" s="16">
+        <v>35</v>
+      </c>
+      <c r="F12" s="16">
+        <v>50</v>
+      </c>
+      <c r="G12" s="16">
+        <v>53</v>
+      </c>
+      <c r="H12">
+        <v>0.61209499999999994</v>
+      </c>
+      <c r="I12">
+        <v>0.59199999999999997</v>
+      </c>
+      <c r="J12">
+        <v>4</v>
+      </c>
+      <c r="K12">
+        <v>40</v>
+      </c>
+      <c r="L12">
+        <v>31</v>
+      </c>
+      <c r="M12">
+        <v>0.10045999999999999</v>
+      </c>
+      <c r="N12">
+        <v>2.4089799999999998E-3</v>
+      </c>
+      <c r="O12">
+        <v>4</v>
+      </c>
+      <c r="P12">
+        <v>60</v>
+      </c>
+      <c r="Q12">
+        <v>71</v>
+      </c>
+      <c r="R12">
+        <v>0.472719</v>
+      </c>
+      <c r="S12">
+        <v>0.108086</v>
+      </c>
+      <c r="T12">
+        <v>4</v>
+      </c>
+      <c r="U12">
+        <v>54</v>
+      </c>
+      <c r="V12">
+        <v>58</v>
+      </c>
+      <c r="W12">
+        <v>0.56790600000000002</v>
+      </c>
+      <c r="X12">
+        <v>0.35607699999999998</v>
+      </c>
+      <c r="Y12">
+        <v>4</v>
+      </c>
+      <c r="Z12">
+        <v>53</v>
+      </c>
+      <c r="AA12">
+        <v>57</v>
+      </c>
+      <c r="AB12">
+        <v>0.58704599999999996</v>
+      </c>
+      <c r="AC12">
+        <v>0.79608800000000002</v>
+      </c>
+      <c r="AD12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30">
+      <c r="A13" s="16">
+        <v>1000</v>
+      </c>
+      <c r="B13" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="C13" s="16">
+        <v>2</v>
+      </c>
+      <c r="D13" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="E13" s="16">
+        <v>44</v>
+      </c>
+      <c r="F13" s="16">
+        <v>60</v>
+      </c>
+      <c r="G13" s="16">
+        <v>95</v>
+      </c>
+      <c r="H13">
+        <v>0.19318299999999999</v>
+      </c>
+      <c r="I13">
+        <v>0.434</v>
+      </c>
+      <c r="J13">
+        <v>4</v>
+      </c>
+      <c r="K13">
+        <v>73</v>
+      </c>
+      <c r="L13">
+        <v>73</v>
+      </c>
+      <c r="M13">
+        <v>8.2965399999999995E-2</v>
+      </c>
+      <c r="N13">
+        <v>4.9998799999999999E-3</v>
+      </c>
+      <c r="O13">
+        <v>4</v>
+      </c>
+      <c r="P13">
+        <v>66</v>
+      </c>
+      <c r="Q13">
+        <v>102</v>
+      </c>
+      <c r="R13">
+        <v>0.176846</v>
+      </c>
+      <c r="S13">
+        <v>0.108361</v>
+      </c>
+      <c r="T13">
+        <v>4</v>
+      </c>
+      <c r="U13">
+        <v>61</v>
+      </c>
+      <c r="V13">
+        <v>97</v>
+      </c>
+      <c r="W13">
+        <v>0.187365</v>
+      </c>
+      <c r="X13">
+        <v>0.41744999999999999</v>
+      </c>
+      <c r="Y13">
+        <v>4</v>
+      </c>
+      <c r="Z13">
+        <v>62</v>
+      </c>
+      <c r="AA13">
+        <v>96</v>
+      </c>
+      <c r="AB13">
+        <v>0.19198399999999999</v>
+      </c>
+      <c r="AC13">
+        <v>0.64459699999999998</v>
+      </c>
+      <c r="AD13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30">
+      <c r="A14" s="16">
+        <v>1000</v>
+      </c>
+      <c r="B14" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="C14" s="16">
+        <v>8</v>
+      </c>
+      <c r="D14" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="E14" s="16">
+        <v>48</v>
+      </c>
+      <c r="F14" s="16">
+        <v>64</v>
+      </c>
+      <c r="G14" s="16">
+        <v>35</v>
+      </c>
+      <c r="H14">
+        <v>0.30381599999999997</v>
+      </c>
+      <c r="I14">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="J14">
+        <v>4</v>
+      </c>
+      <c r="K14">
+        <v>49</v>
+      </c>
+      <c r="L14">
+        <v>21</v>
+      </c>
+      <c r="M14">
+        <v>8.2498299999999997E-2</v>
+      </c>
+      <c r="N14">
+        <v>3.2310500000000001E-3</v>
+      </c>
+      <c r="O14">
+        <v>4</v>
+      </c>
+      <c r="P14">
+        <v>67</v>
+      </c>
+      <c r="Q14">
+        <v>46</v>
+      </c>
+      <c r="R14">
+        <v>0.24377699999999999</v>
+      </c>
+      <c r="S14">
+        <v>0.15236</v>
+      </c>
+      <c r="T14">
+        <v>4</v>
+      </c>
+      <c r="U14">
+        <v>66</v>
+      </c>
+      <c r="V14">
+        <v>40</v>
+      </c>
+      <c r="W14">
+        <v>0.287686</v>
+      </c>
+      <c r="X14">
+        <v>0.54882799999999998</v>
+      </c>
+      <c r="Y14">
+        <v>4</v>
+      </c>
+      <c r="Z14">
+        <v>64</v>
+      </c>
+      <c r="AA14">
+        <v>35</v>
+      </c>
+      <c r="AB14">
+        <v>0.29976399999999997</v>
+      </c>
+      <c r="AC14">
+        <v>1.1551899999999999</v>
+      </c>
+      <c r="AD14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30">
+      <c r="A15" s="16">
+        <v>1000</v>
+      </c>
+      <c r="B15" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="C15" s="16">
+        <v>8</v>
+      </c>
+      <c r="D15" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="E15" s="16">
+        <v>142</v>
+      </c>
+      <c r="F15" s="16">
+        <v>57</v>
+      </c>
+      <c r="G15" s="16">
+        <v>43</v>
+      </c>
+      <c r="H15">
+        <v>1.8854200000000002E-2</v>
+      </c>
+      <c r="I15">
+        <v>0.32600000000000001</v>
+      </c>
+      <c r="J15">
+        <v>4</v>
+      </c>
+      <c r="K15">
+        <v>53</v>
+      </c>
+      <c r="L15">
+        <v>44</v>
+      </c>
+      <c r="M15">
+        <v>1.0001899999999999E-2</v>
+      </c>
+      <c r="N15">
+        <v>2.4659600000000001E-3</v>
+      </c>
+      <c r="O15">
+        <v>4</v>
+      </c>
+      <c r="P15">
+        <v>57</v>
+      </c>
+      <c r="Q15">
+        <v>43</v>
+      </c>
+      <c r="R15">
+        <v>1.8729300000000001E-2</v>
+      </c>
+      <c r="S15">
+        <v>3.1244000000000001E-2</v>
+      </c>
+      <c r="T15">
+        <v>4</v>
+      </c>
+      <c r="U15">
+        <v>57</v>
+      </c>
+      <c r="V15">
+        <v>43</v>
+      </c>
+      <c r="W15">
+        <v>1.8729300000000001E-2</v>
+      </c>
+      <c r="X15">
+        <v>7.8583E-2</v>
+      </c>
+      <c r="Y15">
+        <v>4</v>
+      </c>
+      <c r="Z15">
+        <v>57</v>
+      </c>
+      <c r="AA15">
+        <v>43</v>
+      </c>
+      <c r="AB15">
+        <v>1.8854200000000002E-2</v>
+      </c>
+      <c r="AC15">
+        <v>0.160362</v>
+      </c>
+      <c r="AD15">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:AE15"/>
+  <sheetViews>
+    <sheetView showRuler="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:AE15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:31">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" t="s">
+        <v>43</v>
+      </c>
+      <c r="L3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31">
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" t="s">
+        <v>50</v>
+      </c>
+      <c r="L6" t="s">
+        <v>57</v>
+      </c>
+      <c r="S6" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" t="s">
+        <v>49</v>
+      </c>
+      <c r="J7" t="s">
+        <v>61</v>
+      </c>
+      <c r="K7" t="s">
+        <v>47</v>
+      </c>
+      <c r="L7" t="s">
+        <v>62</v>
+      </c>
+      <c r="M7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N7" t="s">
+        <v>49</v>
+      </c>
+      <c r="O7" t="s">
+        <v>63</v>
+      </c>
+      <c r="P7" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>69</v>
+      </c>
+      <c r="R7" t="s">
+        <v>47</v>
+      </c>
+      <c r="S7" t="s">
+        <v>62</v>
+      </c>
+      <c r="T7" t="s">
+        <v>48</v>
+      </c>
+      <c r="U7" t="s">
+        <v>49</v>
+      </c>
+      <c r="V7" t="s">
+        <v>63</v>
+      </c>
+      <c r="W7" t="s">
+        <v>67</v>
+      </c>
+      <c r="X7" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31">
+      <c r="A8">
+        <v>1000</v>
+      </c>
+      <c r="B8">
+        <v>0.1</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="E8">
+        <v>34</v>
+      </c>
+      <c r="F8">
+        <v>37</v>
+      </c>
+      <c r="G8">
+        <v>55</v>
+      </c>
+      <c r="H8">
+        <v>0.84220700000000004</v>
+      </c>
+      <c r="I8">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="J8">
+        <v>4</v>
+      </c>
+      <c r="K8">
+        <v>60</v>
+      </c>
+      <c r="L8">
+        <v>64</v>
+      </c>
+      <c r="M8">
+        <v>0.75763000000000003</v>
+      </c>
+      <c r="N8">
+        <v>3.1135099999999999E-2</v>
+      </c>
+      <c r="O8">
+        <v>4</v>
+      </c>
+      <c r="P8">
+        <f>M8/H8*100</f>
+        <v>89.957694486034896</v>
+      </c>
+      <c r="Q8">
+        <f>I8/N8</f>
+        <v>29.323817813336078</v>
+      </c>
+      <c r="R8">
+        <v>49</v>
+      </c>
+      <c r="S8">
+        <v>76</v>
+      </c>
+      <c r="T8">
+        <v>0.824627</v>
+      </c>
+      <c r="U8">
+        <v>0.25547599999999998</v>
+      </c>
+      <c r="V8">
+        <v>4</v>
+      </c>
+      <c r="W8">
+        <f>T8/H8*100</f>
+        <v>97.912627180728734</v>
+      </c>
+      <c r="X8">
+        <f>I8/U8</f>
+        <v>3.5737212106029532</v>
+      </c>
+      <c r="Y8">
+        <v>40</v>
+      </c>
+      <c r="Z8">
+        <v>59</v>
+      </c>
+      <c r="AA8">
+        <v>0.83953800000000001</v>
+      </c>
+      <c r="AB8">
+        <v>0.91206200000000004</v>
+      </c>
+      <c r="AC8">
+        <v>4</v>
+      </c>
+      <c r="AD8">
+        <f>AA8/H8*100</f>
+        <v>99.683094536141354</v>
+      </c>
+      <c r="AE8">
+        <f>I8/AB8</f>
+        <v>1.0010284388561304</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31">
+      <c r="A9">
+        <v>1000</v>
+      </c>
+      <c r="B9">
+        <v>0.1</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="E9">
+        <v>44</v>
+      </c>
+      <c r="F9">
+        <v>62</v>
+      </c>
+      <c r="G9">
+        <v>153</v>
+      </c>
+      <c r="H9">
+        <v>0.40223599999999998</v>
+      </c>
+      <c r="I9">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="J9">
+        <v>4</v>
+      </c>
+      <c r="K9">
+        <v>87</v>
+      </c>
+      <c r="L9">
+        <v>116</v>
+      </c>
+      <c r="M9">
+        <v>0.280053</v>
+      </c>
+      <c r="N9">
+        <v>1.5886999999999998E-2</v>
+      </c>
+      <c r="O9">
+        <v>4</v>
+      </c>
+      <c r="P9">
+        <f>M9/H9*100</f>
+        <v>69.624051551825289</v>
+      </c>
+      <c r="Q9">
+        <f>I9/N9</f>
+        <v>53.817586706111918</v>
+      </c>
+      <c r="R9">
+        <v>83</v>
+      </c>
+      <c r="S9">
+        <v>158</v>
+      </c>
+      <c r="T9">
+        <v>0.36341600000000002</v>
+      </c>
+      <c r="U9">
+        <v>8.9420100000000002E-2</v>
+      </c>
+      <c r="V9">
+        <v>4</v>
+      </c>
+      <c r="W9">
+        <f>T9/H9*100</f>
+        <v>90.348949373004899</v>
+      </c>
+      <c r="X9">
+        <f>I9/U9</f>
+        <v>9.561608631616382</v>
+      </c>
+      <c r="Y9">
+        <v>68</v>
+      </c>
+      <c r="Z9">
+        <v>158</v>
+      </c>
+      <c r="AA9">
+        <v>0.39464700000000003</v>
+      </c>
+      <c r="AB9">
+        <v>0.25410100000000002</v>
+      </c>
+      <c r="AC9">
+        <v>4</v>
+      </c>
+      <c r="AD9">
+        <f>AA9/H9*100</f>
+        <v>98.113296671605738</v>
+      </c>
+      <c r="AE9">
+        <f>I9/AB9</f>
+        <v>3.3648037591351465</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31">
+      <c r="A10" s="16">
+        <v>1000</v>
+      </c>
+      <c r="B10" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="C10" s="16">
+        <v>8</v>
+      </c>
+      <c r="D10" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="E10" s="16">
+        <v>51</v>
+      </c>
+      <c r="F10" s="16">
+        <v>58</v>
+      </c>
+      <c r="G10" s="16">
+        <v>30</v>
+      </c>
+      <c r="H10">
+        <v>-1.98088E-3</v>
+      </c>
+      <c r="I10">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="J10">
+        <v>4</v>
+      </c>
+      <c r="K10">
+        <v>76</v>
+      </c>
+      <c r="L10">
+        <v>46</v>
+      </c>
+      <c r="M10">
+        <v>-1.8992200000000001E-3</v>
+      </c>
+      <c r="N10">
+        <v>2.4927899999999999E-2</v>
+      </c>
+      <c r="O10">
+        <v>4</v>
+      </c>
+      <c r="P10">
+        <f t="shared" ref="P10:P15" si="0">M10/H10*100</f>
+        <v>95.877589758087325</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" ref="Q10:Q15" si="1">I10/N10</f>
+        <v>29.364687759498395</v>
+      </c>
+      <c r="R10">
+        <v>65</v>
+      </c>
+      <c r="S10">
+        <v>39</v>
+      </c>
+      <c r="T10">
+        <v>-1.9928599999999999E-3</v>
+      </c>
+      <c r="U10">
+        <v>0.159332</v>
+      </c>
+      <c r="V10">
+        <v>4</v>
+      </c>
+      <c r="W10">
+        <f>T10/H10*100</f>
+        <v>100.60478171317797</v>
+      </c>
+      <c r="X10">
+        <f t="shared" ref="X10:X15" si="2">I10/U10</f>
+        <v>4.5941807044410412</v>
+      </c>
+      <c r="Y10">
+        <v>61</v>
+      </c>
+      <c r="Z10">
+        <v>35</v>
+      </c>
+      <c r="AA10">
+        <v>-2.2480199999999999E-3</v>
+      </c>
+      <c r="AB10">
+        <v>0.54999600000000004</v>
+      </c>
+      <c r="AC10">
+        <v>4</v>
+      </c>
+      <c r="AD10">
+        <f>AA10/H10*100</f>
+        <v>113.48592544727596</v>
+      </c>
+      <c r="AE10">
+        <f t="shared" ref="AE10:AE15" si="3">I10/AB10</f>
+        <v>1.3309187703183294</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31">
+      <c r="A11" s="16">
+        <v>1000</v>
+      </c>
+      <c r="B11" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="C11" s="16">
+        <v>8</v>
+      </c>
+      <c r="D11" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="E11" s="16">
+        <v>130</v>
+      </c>
+      <c r="F11" s="16">
+        <v>74</v>
+      </c>
+      <c r="G11" s="16">
+        <v>68</v>
+      </c>
+      <c r="H11">
+        <v>0.03</v>
+      </c>
+      <c r="I11">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="J11">
+        <v>4</v>
+      </c>
+      <c r="K11">
+        <v>74</v>
+      </c>
+      <c r="L11">
+        <v>56</v>
+      </c>
+      <c r="M11">
+        <v>1.9789500000000002E-2</v>
+      </c>
+      <c r="N11">
+        <v>5.0818900000000004E-3</v>
+      </c>
+      <c r="O11">
+        <v>4</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="0"/>
+        <v>65.965000000000003</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="1"/>
+        <v>70.446231618551352</v>
+      </c>
+      <c r="R11">
+        <v>79</v>
+      </c>
+      <c r="S11">
+        <v>66</v>
+      </c>
+      <c r="T11">
+        <v>2.77805E-2</v>
+      </c>
+      <c r="U11">
+        <v>1.5967100000000001E-2</v>
+      </c>
+      <c r="V11">
+        <v>4</v>
+      </c>
+      <c r="W11">
+        <f>T11/H11*100</f>
+        <v>92.601666666666674</v>
+      </c>
+      <c r="X11">
+        <f t="shared" si="2"/>
+        <v>22.42110339385361</v>
+      </c>
+      <c r="Y11">
+        <v>79</v>
+      </c>
+      <c r="Z11">
+        <v>72</v>
+      </c>
+      <c r="AA11">
+        <v>3.0200299999999999E-2</v>
+      </c>
+      <c r="AB11">
+        <v>4.1770000000000002E-2</v>
+      </c>
+      <c r="AC11">
+        <v>4</v>
+      </c>
+      <c r="AD11">
+        <f>AA11/H11*100</f>
+        <v>100.66766666666666</v>
+      </c>
+      <c r="AE11">
+        <f t="shared" si="3"/>
+        <v>8.5707445535073017</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31">
+      <c r="A12" s="16">
+        <v>1000</v>
+      </c>
+      <c r="B12" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="C12" s="16">
+        <v>2</v>
+      </c>
+      <c r="D12" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="E12" s="16">
+        <v>35</v>
+      </c>
+      <c r="F12" s="16">
+        <v>50</v>
+      </c>
+      <c r="G12" s="16">
+        <v>53</v>
+      </c>
+      <c r="H12">
+        <v>0.61209499999999994</v>
+      </c>
+      <c r="I12">
+        <v>0.59199999999999997</v>
+      </c>
+      <c r="J12">
+        <v>4</v>
+      </c>
+      <c r="K12">
+        <v>69</v>
+      </c>
+      <c r="L12">
+        <v>67</v>
+      </c>
+      <c r="M12">
+        <v>0.46099600000000002</v>
+      </c>
+      <c r="N12">
+        <v>1.3454000000000001E-2</v>
+      </c>
+      <c r="O12">
+        <v>4</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="0"/>
+        <v>75.314452821865899</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="1"/>
+        <v>44.001783856102271</v>
+      </c>
+      <c r="R12">
+        <v>64</v>
+      </c>
+      <c r="S12">
+        <v>73</v>
+      </c>
+      <c r="T12">
+        <v>0.57736399999999999</v>
+      </c>
+      <c r="U12">
+        <v>9.0029999999999999E-2</v>
+      </c>
+      <c r="V12">
+        <v>4</v>
+      </c>
+      <c r="W12">
+        <f>T12/H12*100</f>
+        <v>94.325880786479232</v>
+      </c>
+      <c r="X12">
+        <f t="shared" si="2"/>
+        <v>6.5755859158058421</v>
+      </c>
+      <c r="Y12">
+        <v>55</v>
+      </c>
+      <c r="Z12">
+        <v>60</v>
+      </c>
+      <c r="AA12">
+        <v>0.60531000000000001</v>
+      </c>
+      <c r="AB12">
+        <v>0.32089499999999999</v>
+      </c>
+      <c r="AC12">
+        <v>4</v>
+      </c>
+      <c r="AD12">
+        <f>AA12/H12*100</f>
+        <v>98.891511938506298</v>
+      </c>
+      <c r="AE12">
+        <f t="shared" si="3"/>
+        <v>1.8448402125305785</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31">
+      <c r="A13" s="16">
+        <v>1000</v>
+      </c>
+      <c r="B13" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="C13" s="16">
+        <v>2</v>
+      </c>
+      <c r="D13" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="E13" s="16">
+        <v>44</v>
+      </c>
+      <c r="F13" s="16">
+        <v>60</v>
+      </c>
+      <c r="G13" s="16">
+        <v>95</v>
+      </c>
+      <c r="H13">
+        <v>0.19318299999999999</v>
+      </c>
+      <c r="I13">
+        <v>0.434</v>
+      </c>
+      <c r="J13">
+        <v>4</v>
+      </c>
+      <c r="K13">
+        <v>92</v>
+      </c>
+      <c r="L13">
+        <v>93</v>
+      </c>
+      <c r="M13">
+        <v>0.109227</v>
+      </c>
+      <c r="N13">
+        <v>6.2849500000000001E-3</v>
+      </c>
+      <c r="O13">
+        <v>4</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="0"/>
+        <v>56.540689398135449</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="1"/>
+        <v>69.053850865957557</v>
+      </c>
+      <c r="R13">
+        <v>85</v>
+      </c>
+      <c r="S13">
+        <v>102</v>
+      </c>
+      <c r="T13">
+        <v>0.15245600000000001</v>
+      </c>
+      <c r="U13">
+        <v>2.3877900000000001E-2</v>
+      </c>
+      <c r="V13">
+        <v>4</v>
+      </c>
+      <c r="W13">
+        <f>T13/H13*100</f>
+        <v>78.917917208035917</v>
+      </c>
+      <c r="X13">
+        <f t="shared" si="2"/>
+        <v>18.175802729720786</v>
+      </c>
+      <c r="Y13">
+        <v>77</v>
+      </c>
+      <c r="Z13">
+        <v>106</v>
+      </c>
+      <c r="AA13">
+        <v>0.16934299999999999</v>
+      </c>
+      <c r="AB13">
+        <v>6.83589E-2</v>
+      </c>
+      <c r="AC13">
+        <v>4</v>
+      </c>
+      <c r="AD13">
+        <f>AA13/H13*100</f>
+        <v>87.65936961326824</v>
+      </c>
+      <c r="AE13">
+        <f t="shared" si="3"/>
+        <v>6.3488441153968243</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31">
+      <c r="A14" s="16">
+        <v>1000</v>
+      </c>
+      <c r="B14" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="C14" s="16">
+        <v>8</v>
+      </c>
+      <c r="D14" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="E14" s="16">
+        <v>48</v>
+      </c>
+      <c r="F14" s="16">
+        <v>64</v>
+      </c>
+      <c r="G14" s="16">
+        <v>35</v>
+      </c>
+      <c r="H14">
+        <v>0.30381599999999997</v>
+      </c>
+      <c r="I14">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="J14">
+        <v>4</v>
+      </c>
+      <c r="K14">
+        <v>79</v>
+      </c>
+      <c r="L14">
+        <v>59</v>
+      </c>
+      <c r="M14">
+        <v>0.23926600000000001</v>
+      </c>
+      <c r="N14">
+        <v>1.1403099999999999E-2</v>
+      </c>
+      <c r="O14">
+        <v>4</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="0"/>
+        <v>78.75358769781711</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="1"/>
+        <v>41.392252983837729</v>
+      </c>
+      <c r="R14">
+        <v>74</v>
+      </c>
+      <c r="S14">
+        <v>55</v>
+      </c>
+      <c r="T14">
+        <v>0.292717</v>
+      </c>
+      <c r="U14">
+        <v>6.3992999999999994E-2</v>
+      </c>
+      <c r="V14">
+        <v>4</v>
+      </c>
+      <c r="W14">
+        <f>T14/H14*100</f>
+        <v>96.346802011743961</v>
+      </c>
+      <c r="X14">
+        <f t="shared" si="2"/>
+        <v>7.3758067288609697</v>
+      </c>
+      <c r="Y14">
+        <v>69</v>
+      </c>
+      <c r="Z14">
+        <v>46</v>
+      </c>
+      <c r="AA14">
+        <v>0.30113499999999999</v>
+      </c>
+      <c r="AB14">
+        <v>0.20505200000000001</v>
+      </c>
+      <c r="AC14">
+        <v>4</v>
+      </c>
+      <c r="AD14">
+        <f>AA14/H14*100</f>
+        <v>99.117557995628943</v>
+      </c>
+      <c r="AE14">
+        <f t="shared" si="3"/>
+        <v>2.3018551391842066</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31">
+      <c r="A15" s="16">
+        <v>1000</v>
+      </c>
+      <c r="B15" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="C15" s="16">
+        <v>8</v>
+      </c>
+      <c r="D15" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="E15" s="16">
+        <v>142</v>
+      </c>
+      <c r="F15" s="16">
+        <v>57</v>
+      </c>
+      <c r="G15" s="16">
+        <v>43</v>
+      </c>
+      <c r="H15">
+        <v>1.8854200000000002E-2</v>
+      </c>
+      <c r="I15">
+        <v>0.32600000000000001</v>
+      </c>
+      <c r="J15">
+        <v>4</v>
+      </c>
+      <c r="K15">
+        <v>58</v>
+      </c>
+      <c r="L15">
+        <v>46</v>
+      </c>
+      <c r="M15">
+        <v>1.28416E-2</v>
+      </c>
+      <c r="N15">
+        <v>4.5001499999999996E-3</v>
+      </c>
+      <c r="O15">
+        <v>4</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="0"/>
+        <v>68.11002323089815</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="1"/>
+        <v>72.442029710120778</v>
+      </c>
+      <c r="R15">
+        <v>61</v>
+      </c>
+      <c r="S15">
+        <v>49</v>
+      </c>
+      <c r="T15">
+        <v>1.6754499999999999E-2</v>
+      </c>
+      <c r="U15">
+        <v>1.0696900000000001E-2</v>
+      </c>
+      <c r="V15">
+        <v>4</v>
+      </c>
+      <c r="W15">
+        <f>T15/H15*100</f>
+        <v>88.863489302118353</v>
+      </c>
+      <c r="X15">
+        <f t="shared" si="2"/>
+        <v>30.47611924950219</v>
+      </c>
+      <c r="Y15">
+        <v>59</v>
+      </c>
+      <c r="Z15">
+        <v>45</v>
+      </c>
+      <c r="AA15">
+        <v>1.7733599999999999E-2</v>
+      </c>
+      <c r="AB15">
+        <v>3.4079999999999999E-2</v>
+      </c>
+      <c r="AC15">
+        <v>4</v>
+      </c>
+      <c r="AD15">
+        <f>AA15/H15*100</f>
+        <v>94.056496695696438</v>
+      </c>
+      <c r="AE15">
+        <f t="shared" si="3"/>
+        <v>9.5657276995305178</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:AO12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="AO1" sqref="AO1:AO1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.1640625" customWidth="1"/>
+    <col min="5" max="5" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.83203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.1640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.83203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.1640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.83203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.1640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="10.83203125" style="18"/>
+    <col min="40" max="40" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="10.83203125" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:41">
+      <c r="I3" t="s">
+        <v>45</v>
+      </c>
+      <c r="O3" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="U3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" t="s">
+        <v>47</v>
+      </c>
+      <c r="M4" t="s">
+        <v>62</v>
+      </c>
+      <c r="O4" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q4" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="S4" t="s">
+        <v>47</v>
+      </c>
+      <c r="U4" t="s">
+        <v>62</v>
+      </c>
+      <c r="W4" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y4" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE4" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG4" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>47</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM4" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="AO4" s="18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41">
+      <c r="A5">
+        <v>1000</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5">
+        <v>0.1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I5">
+        <v>34</v>
+      </c>
+      <c r="J5" t="s">
+        <v>70</v>
+      </c>
+      <c r="K5">
+        <v>37</v>
+      </c>
+      <c r="L5" t="s">
+        <v>70</v>
+      </c>
+      <c r="M5">
+        <v>55</v>
+      </c>
+      <c r="N5" t="s">
+        <v>70</v>
+      </c>
+      <c r="O5" s="18">
+        <v>0.84220700000000004</v>
+      </c>
+      <c r="P5" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q5" s="18">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="R5" t="s">
+        <v>70</v>
+      </c>
+      <c r="S5">
+        <v>60</v>
+      </c>
+      <c r="T5" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="U5">
+        <v>64</v>
+      </c>
+      <c r="V5" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="W5" s="18">
+        <v>0.75763000000000003</v>
+      </c>
+      <c r="X5" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y5" s="18">
+        <v>3.1135099999999999E-2</v>
+      </c>
+      <c r="Z5" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA5">
+        <v>49</v>
+      </c>
+      <c r="AB5" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC5">
+        <v>76</v>
+      </c>
+      <c r="AD5" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE5" s="18">
+        <v>0.824627</v>
+      </c>
+      <c r="AF5" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG5" s="18">
+        <v>0.25547599999999998</v>
+      </c>
+      <c r="AH5" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI5">
+        <v>40</v>
+      </c>
+      <c r="AJ5" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AK5">
+        <v>59</v>
+      </c>
+      <c r="AL5" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM5" s="18">
+        <v>0.83953800000000001</v>
+      </c>
+      <c r="AN5" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AO5" s="18">
+        <v>0.91206200000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41">
+      <c r="A6">
+        <v>1000</v>
+      </c>
+      <c r="B6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6">
+        <v>0.1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>70</v>
+      </c>
+      <c r="I6">
+        <v>44</v>
+      </c>
+      <c r="J6" t="s">
+        <v>70</v>
+      </c>
+      <c r="K6">
+        <v>62</v>
+      </c>
+      <c r="L6" t="s">
+        <v>70</v>
+      </c>
+      <c r="M6">
+        <v>153</v>
+      </c>
+      <c r="N6" t="s">
+        <v>70</v>
+      </c>
+      <c r="O6" s="18">
+        <v>0.40223599999999998</v>
+      </c>
+      <c r="P6" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q6" s="18">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="R6" t="s">
+        <v>70</v>
+      </c>
+      <c r="S6">
+        <v>87</v>
+      </c>
+      <c r="T6" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="U6">
+        <v>116</v>
+      </c>
+      <c r="V6" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="W6" s="18">
+        <v>0.280053</v>
+      </c>
+      <c r="X6" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y6" s="18">
+        <v>1.5886999999999998E-2</v>
+      </c>
+      <c r="Z6" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA6">
+        <v>83</v>
+      </c>
+      <c r="AB6" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC6">
+        <v>158</v>
+      </c>
+      <c r="AD6" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE6" s="18">
+        <v>0.36341600000000002</v>
+      </c>
+      <c r="AF6" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG6" s="18">
+        <v>8.9420100000000002E-2</v>
+      </c>
+      <c r="AH6" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI6">
+        <v>68</v>
+      </c>
+      <c r="AJ6" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AK6">
+        <v>158</v>
+      </c>
+      <c r="AL6" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM6" s="18">
+        <v>0.39464700000000003</v>
+      </c>
+      <c r="AN6" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AO6" s="18">
+        <v>0.25410100000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41">
+      <c r="A7" s="16">
+        <v>1000</v>
+      </c>
+      <c r="B7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="16">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>70</v>
+      </c>
+      <c r="I7" s="16">
+        <v>51</v>
+      </c>
+      <c r="J7" t="s">
+        <v>70</v>
+      </c>
+      <c r="K7" s="16">
+        <v>58</v>
+      </c>
+      <c r="L7" t="s">
+        <v>70</v>
+      </c>
+      <c r="M7" s="16">
+        <v>30</v>
+      </c>
+      <c r="N7" t="s">
+        <v>70</v>
+      </c>
+      <c r="O7" s="18">
+        <v>-1.98088E-3</v>
+      </c>
+      <c r="P7" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q7" s="18">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="R7" t="s">
+        <v>70</v>
+      </c>
+      <c r="S7">
+        <v>76</v>
+      </c>
+      <c r="T7" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="U7">
+        <v>46</v>
+      </c>
+      <c r="V7" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="W7" s="18">
+        <v>-1.8992200000000001E-3</v>
+      </c>
+      <c r="X7" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y7" s="18">
+        <v>2.4927899999999999E-2</v>
+      </c>
+      <c r="Z7" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA7">
+        <v>65</v>
+      </c>
+      <c r="AB7" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC7">
+        <v>39</v>
+      </c>
+      <c r="AD7" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE7" s="18">
+        <v>-1.9928599999999999E-3</v>
+      </c>
+      <c r="AF7" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG7" s="18">
+        <v>0.159332</v>
+      </c>
+      <c r="AH7" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI7">
+        <v>61</v>
+      </c>
+      <c r="AJ7" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AK7">
+        <v>35</v>
+      </c>
+      <c r="AL7" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM7" s="18">
+        <v>-2.2480199999999999E-3</v>
+      </c>
+      <c r="AN7" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AO7" s="18">
+        <v>0.54999600000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41">
+      <c r="A8" s="16">
+        <v>1000</v>
+      </c>
+      <c r="B8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="16">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G8" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="H8" t="s">
+        <v>70</v>
+      </c>
+      <c r="I8" s="16">
+        <v>130</v>
+      </c>
+      <c r="J8" t="s">
+        <v>70</v>
+      </c>
+      <c r="K8" s="16">
+        <v>74</v>
+      </c>
+      <c r="L8" t="s">
+        <v>70</v>
+      </c>
+      <c r="M8" s="16">
+        <v>68</v>
+      </c>
+      <c r="N8" t="s">
+        <v>70</v>
+      </c>
+      <c r="O8" s="18">
+        <v>3.02247E-2</v>
+      </c>
+      <c r="P8" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q8" s="18">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="R8" t="s">
+        <v>70</v>
+      </c>
+      <c r="S8">
+        <v>74</v>
+      </c>
+      <c r="T8" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="U8">
+        <v>56</v>
+      </c>
+      <c r="V8" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="W8" s="18">
+        <v>1.9789500000000002E-2</v>
+      </c>
+      <c r="X8" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y8" s="18">
+        <v>5.0818900000000004E-3</v>
+      </c>
+      <c r="Z8" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA8">
+        <v>79</v>
+      </c>
+      <c r="AB8" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC8">
+        <v>66</v>
+      </c>
+      <c r="AD8" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE8" s="18">
+        <v>2.77805E-2</v>
+      </c>
+      <c r="AF8" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG8" s="18">
+        <v>1.5967100000000001E-2</v>
+      </c>
+      <c r="AH8" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI8">
+        <v>79</v>
+      </c>
+      <c r="AJ8" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AK8">
+        <v>72</v>
+      </c>
+      <c r="AL8" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM8" s="18">
+        <v>3.0200299999999999E-2</v>
+      </c>
+      <c r="AN8" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AO8" s="18">
+        <v>4.1770000000000002E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41">
+      <c r="A9" s="16">
+        <v>1000</v>
+      </c>
+      <c r="B9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="16">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I9" s="16">
+        <v>35</v>
+      </c>
+      <c r="J9" t="s">
+        <v>70</v>
+      </c>
+      <c r="K9" s="16">
+        <v>50</v>
+      </c>
+      <c r="L9" t="s">
+        <v>70</v>
+      </c>
+      <c r="M9" s="16">
+        <v>53</v>
+      </c>
+      <c r="N9" t="s">
+        <v>70</v>
+      </c>
+      <c r="O9" s="18">
+        <v>0.61209499999999994</v>
+      </c>
+      <c r="P9" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q9" s="18">
+        <v>0.59199999999999997</v>
+      </c>
+      <c r="R9" t="s">
+        <v>70</v>
+      </c>
+      <c r="S9">
+        <v>69</v>
+      </c>
+      <c r="T9" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="U9">
+        <v>67</v>
+      </c>
+      <c r="V9" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="W9" s="18">
+        <v>0.46099600000000002</v>
+      </c>
+      <c r="X9" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y9" s="18">
+        <v>1.3454000000000001E-2</v>
+      </c>
+      <c r="Z9" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA9">
+        <v>64</v>
+      </c>
+      <c r="AB9" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC9">
+        <v>73</v>
+      </c>
+      <c r="AD9" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE9" s="18">
+        <v>0.57736399999999999</v>
+      </c>
+      <c r="AF9" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG9" s="18">
+        <v>9.0029999999999999E-2</v>
+      </c>
+      <c r="AH9" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI9">
+        <v>55</v>
+      </c>
+      <c r="AJ9" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AK9">
+        <v>60</v>
+      </c>
+      <c r="AL9" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM9" s="18">
+        <v>0.60531000000000001</v>
+      </c>
+      <c r="AN9" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AO9" s="18">
+        <v>0.32089499999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41">
+      <c r="A10" s="16">
+        <v>1000</v>
+      </c>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="16">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="H10" t="s">
+        <v>70</v>
+      </c>
+      <c r="I10" s="16">
+        <v>44</v>
+      </c>
+      <c r="J10" t="s">
+        <v>70</v>
+      </c>
+      <c r="K10" s="16">
+        <v>60</v>
+      </c>
+      <c r="L10" t="s">
+        <v>70</v>
+      </c>
+      <c r="M10" s="16">
+        <v>95</v>
+      </c>
+      <c r="N10" t="s">
+        <v>70</v>
+      </c>
+      <c r="O10" s="18">
+        <v>0.19318299999999999</v>
+      </c>
+      <c r="P10" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q10" s="18">
+        <v>0.434</v>
+      </c>
+      <c r="R10" t="s">
+        <v>70</v>
+      </c>
+      <c r="S10">
+        <v>92</v>
+      </c>
+      <c r="T10" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="U10">
+        <v>93</v>
+      </c>
+      <c r="V10" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="W10" s="18">
+        <v>0.109227</v>
+      </c>
+      <c r="X10" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y10" s="18">
+        <v>6.2849500000000001E-3</v>
+      </c>
+      <c r="Z10" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA10">
+        <v>85</v>
+      </c>
+      <c r="AB10" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC10">
+        <v>102</v>
+      </c>
+      <c r="AD10" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE10" s="18">
+        <v>0.15245600000000001</v>
+      </c>
+      <c r="AF10" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG10" s="18">
+        <v>2.3877900000000001E-2</v>
+      </c>
+      <c r="AH10" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI10">
+        <v>77</v>
+      </c>
+      <c r="AJ10" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AK10">
+        <v>106</v>
+      </c>
+      <c r="AL10" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM10" s="18">
+        <v>0.16934299999999999</v>
+      </c>
+      <c r="AN10" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AO10" s="18">
+        <v>6.83589E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41">
+      <c r="A11" s="16">
+        <v>1000</v>
+      </c>
+      <c r="B11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="16">
+        <v>8</v>
+      </c>
+      <c r="F11" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>70</v>
+      </c>
+      <c r="I11" s="16">
+        <v>48</v>
+      </c>
+      <c r="J11" t="s">
+        <v>70</v>
+      </c>
+      <c r="K11" s="16">
+        <v>64</v>
+      </c>
+      <c r="L11" t="s">
+        <v>70</v>
+      </c>
+      <c r="M11" s="16">
+        <v>35</v>
+      </c>
+      <c r="N11" t="s">
+        <v>70</v>
+      </c>
+      <c r="O11" s="18">
+        <v>0.30381599999999997</v>
+      </c>
+      <c r="P11" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q11" s="18">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="R11" t="s">
+        <v>70</v>
+      </c>
+      <c r="S11">
+        <v>79</v>
+      </c>
+      <c r="T11" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="U11">
+        <v>59</v>
+      </c>
+      <c r="V11" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="W11" s="18">
+        <v>0.23926600000000001</v>
+      </c>
+      <c r="X11" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y11" s="18">
+        <v>1.1403099999999999E-2</v>
+      </c>
+      <c r="Z11" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA11">
+        <v>74</v>
+      </c>
+      <c r="AB11" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC11">
+        <v>55</v>
+      </c>
+      <c r="AD11" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE11" s="18">
+        <v>0.292717</v>
+      </c>
+      <c r="AF11" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG11" s="18">
+        <v>6.3992999999999994E-2</v>
+      </c>
+      <c r="AH11" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI11">
+        <v>69</v>
+      </c>
+      <c r="AJ11" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AK11">
+        <v>46</v>
+      </c>
+      <c r="AL11" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM11" s="18">
+        <v>0.30113499999999999</v>
+      </c>
+      <c r="AN11" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AO11" s="18">
+        <v>0.20505200000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41">
+      <c r="A12" s="16">
+        <v>1000</v>
+      </c>
+      <c r="B12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="16">
+        <v>8</v>
+      </c>
+      <c r="F12" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="H12" t="s">
+        <v>70</v>
+      </c>
+      <c r="I12" s="16">
+        <v>142</v>
+      </c>
+      <c r="J12" t="s">
+        <v>70</v>
+      </c>
+      <c r="K12" s="16">
+        <v>57</v>
+      </c>
+      <c r="L12" t="s">
+        <v>70</v>
+      </c>
+      <c r="M12" s="16">
+        <v>43</v>
+      </c>
+      <c r="N12" t="s">
+        <v>70</v>
+      </c>
+      <c r="O12" s="18">
+        <v>1.8854200000000002E-2</v>
+      </c>
+      <c r="P12" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q12" s="18">
+        <v>0.32600000000000001</v>
+      </c>
+      <c r="R12" t="s">
+        <v>70</v>
+      </c>
+      <c r="S12">
+        <v>58</v>
+      </c>
+      <c r="T12" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="U12">
+        <v>46</v>
+      </c>
+      <c r="V12" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="W12" s="18">
+        <v>1.28416E-2</v>
+      </c>
+      <c r="X12" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y12" s="18">
+        <v>4.5001499999999996E-3</v>
+      </c>
+      <c r="Z12" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA12">
+        <v>61</v>
+      </c>
+      <c r="AB12" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC12">
+        <v>49</v>
+      </c>
+      <c r="AD12" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE12" s="18">
+        <v>1.6754499999999999E-2</v>
+      </c>
+      <c r="AF12" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG12" s="18">
+        <v>1.0696900000000001E-2</v>
+      </c>
+      <c r="AH12" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI12">
+        <v>59</v>
+      </c>
+      <c r="AJ12" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AK12">
+        <v>45</v>
+      </c>
+      <c r="AL12" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM12" s="18">
+        <v>1.7733599999999999E-2</v>
+      </c>
+      <c r="AN12" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AO12" s="18">
+        <v>3.4079999999999999E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding more analysis stuff
</commit_message>
<xml_diff>
--- a/plots-data.xlsx
+++ b/plots-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="340" windowWidth="32980" windowHeight="17540" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="220" yWindow="1100" windowWidth="32980" windowHeight="17540" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="86">
   <si>
     <t>brock200_2</t>
   </si>
@@ -256,6 +256,9 @@
     <t>OurAlgo(c=2)</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>C5%Cfinder</t>
   </si>
   <si>
@@ -270,14 +273,57 @@
   <si>
     <t>&amp;</t>
   </si>
+  <si>
+    <t>\\</t>
+  </si>
+  <si>
+    <t>time-clique</t>
+  </si>
+  <si>
+    <t>total time</t>
+  </si>
+  <si>
+    <t>%time-clique</t>
+  </si>
+  <si>
+    <t>facebook_network</t>
+  </si>
+  <si>
+    <t>twitter_network</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Cfinder</t>
+  </si>
+  <si>
+    <t>SharedNodes</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Time-clique</t>
+  </si>
+  <si>
+    <t>Total time</t>
+  </si>
+  <si>
+    <t>c=0</t>
+  </si>
+  <si>
+    <t>c=5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -365,7 +411,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="191">
+  <cellStyleXfs count="361">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -557,8 +603,178 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -586,8 +802,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="191">
+  <cellStyles count="361">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -683,6 +902,91 @@
     <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="324" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="326" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="328" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="330" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="332" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="334" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="338" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="340" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="342" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="344" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="346" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="348" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="350" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="352" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="354" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="356" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="358" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="360" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -778,6 +1082,91 @@
     <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="321" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="323" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="325" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="327" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="329" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="331" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="333" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="335" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="337" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="339" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="341" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="343" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="345" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="347" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="349" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="351" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="353" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="355" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="357" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="359" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1649,6 +2038,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1705,6 +2095,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
@@ -1726,6 +2117,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -9361,6 +9753,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -9417,6 +9810,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
@@ -9438,6 +9832,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -11849,6 +12244,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -11900,6 +12296,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
@@ -11921,6 +12318,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -12396,6 +12794,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -12452,6 +12851,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
@@ -12473,6 +12873,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -12983,6 +13384,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -13698,6 +14100,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -14413,6 +14816,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -15291,6 +15695,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -15357,6 +15762,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
@@ -15388,6 +15794,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -17071,7 +17478,7 @@
   <dimension ref="A1:R41"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -19224,6 +19631,7 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -20780,8 +21188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AD15"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="M1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="Q17" sqref="A1:XFD1048576"/>
+    <sheetView showRuler="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -21693,10 +22101,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AE15"/>
+  <dimension ref="A2:AE26"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:AE15"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -21811,10 +22219,10 @@
         <v>63</v>
       </c>
       <c r="P7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="Q7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="R7" t="s">
         <v>47</v>
@@ -21832,10 +22240,10 @@
         <v>63</v>
       </c>
       <c r="W7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="X7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Y7" t="s">
         <v>47</v>
@@ -21853,10 +22261,10 @@
         <v>63</v>
       </c>
       <c r="AD7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AE7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:31">
@@ -22665,6 +23073,323 @@
       <c r="AE15">
         <f t="shared" si="3"/>
         <v>9.5657276995305178</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31">
+      <c r="P16">
+        <f>SUM(P8:P15)/8</f>
+        <v>75.017886118083013</v>
+      </c>
+      <c r="Q16">
+        <f>SUM(Q8:Q15)/8</f>
+        <v>51.230280164189516</v>
+      </c>
+      <c r="W16">
+        <f>SUM(W8:W15)/8</f>
+        <v>92.490264280244475</v>
+      </c>
+      <c r="X16">
+        <f>SUM(X8:X15)/8</f>
+        <v>12.844241070550471</v>
+      </c>
+      <c r="AD16">
+        <f>SUM(AD8:AD15)/8</f>
+        <v>98.959364945598693</v>
+      </c>
+      <c r="AE16">
+        <f>SUM(AE8:AE15)/8</f>
+        <v>4.2910953360573796</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="C19" t="s">
+        <v>79</v>
+      </c>
+      <c r="F19" t="s">
+        <v>84</v>
+      </c>
+      <c r="J19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" t="s">
+        <v>80</v>
+      </c>
+      <c r="G20" t="s">
+        <v>82</v>
+      </c>
+      <c r="H20" t="s">
+        <v>83</v>
+      </c>
+      <c r="I20" t="s">
+        <v>47</v>
+      </c>
+      <c r="J20" t="s">
+        <v>80</v>
+      </c>
+      <c r="K20" t="s">
+        <v>82</v>
+      </c>
+      <c r="L20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>4132</v>
+      </c>
+      <c r="C21">
+        <f>3228+1014+473+230+108+67+22+14+8+7+4+4+1</f>
+        <v>5180</v>
+      </c>
+      <c r="D21">
+        <v>68.459999999999994</v>
+      </c>
+      <c r="E21">
+        <v>3081</v>
+      </c>
+      <c r="F21">
+        <v>3937</v>
+      </c>
+      <c r="G21">
+        <v>0.13043299999999999</v>
+      </c>
+      <c r="H21">
+        <v>14.000299999999999</v>
+      </c>
+      <c r="I21">
+        <v>3070</v>
+      </c>
+      <c r="J21">
+        <v>4460</v>
+      </c>
+      <c r="K21">
+        <v>0.91746499999999997</v>
+      </c>
+      <c r="L21">
+        <v>417.15100000000001</v>
+      </c>
+      <c r="M21">
+        <f>D21/G21*0.95</f>
+        <v>498.62381452546515</v>
+      </c>
+      <c r="N21">
+        <f>D21/K21*0.95</f>
+        <v>70.887717787599527</v>
+      </c>
+      <c r="O21">
+        <f>D21/H21</f>
+        <v>4.8898952165310741</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22">
+        <v>3947</v>
+      </c>
+      <c r="F22">
+        <v>4229</v>
+      </c>
+      <c r="G22">
+        <v>9.5930799999999997E-2</v>
+      </c>
+      <c r="H22">
+        <v>7.5047800000000002</v>
+      </c>
+      <c r="I22">
+        <v>2518</v>
+      </c>
+      <c r="J22">
+        <v>3899</v>
+      </c>
+      <c r="K22">
+        <v>0.81851499999999999</v>
+      </c>
+      <c r="L22">
+        <v>353.23599999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23">
+        <v>3675</v>
+      </c>
+      <c r="C23">
+        <f>2951+1096+228+29+4</f>
+        <v>4308</v>
+      </c>
+      <c r="D23">
+        <v>9.67</v>
+      </c>
+      <c r="E23">
+        <v>2185</v>
+      </c>
+      <c r="F23">
+        <v>1799</v>
+      </c>
+      <c r="G23">
+        <v>3.9567900000000003E-2</v>
+      </c>
+      <c r="H23">
+        <v>1.1317200000000001</v>
+      </c>
+      <c r="I23">
+        <v>3222</v>
+      </c>
+      <c r="J23">
+        <v>4154</v>
+      </c>
+      <c r="K23">
+        <v>0.300431</v>
+      </c>
+      <c r="L23">
+        <v>95.595799999999997</v>
+      </c>
+      <c r="M23">
+        <f>D23/G23*0.95</f>
+        <v>232.17052206460286</v>
+      </c>
+      <c r="N23">
+        <f>D23/K23*0.95</f>
+        <v>30.577736651677093</v>
+      </c>
+      <c r="O23">
+        <f>D23/H23</f>
+        <v>8.5445163114551299</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24">
+        <v>29</v>
+      </c>
+      <c r="C24">
+        <v>29</v>
+      </c>
+      <c r="D24">
+        <v>3.42</v>
+      </c>
+      <c r="E24">
+        <v>38</v>
+      </c>
+      <c r="F24">
+        <v>46</v>
+      </c>
+      <c r="G24">
+        <v>2.30503E-3</v>
+      </c>
+      <c r="H24">
+        <v>1.1018E-2</v>
+      </c>
+      <c r="I24">
+        <v>19</v>
+      </c>
+      <c r="J24">
+        <v>27</v>
+      </c>
+      <c r="K24">
+        <v>2.29871E-2</v>
+      </c>
+      <c r="L24">
+        <v>0.25202200000000002</v>
+      </c>
+      <c r="M24">
+        <f>D24/G24*0.95</f>
+        <v>1409.5261233042518</v>
+      </c>
+      <c r="N24">
+        <f>D24/K24*0.95</f>
+        <v>141.34014294974136</v>
+      </c>
+      <c r="O24">
+        <f>D24/H24</f>
+        <v>310.40116173534216</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25">
+        <v>22</v>
+      </c>
+      <c r="F25">
+        <v>26</v>
+      </c>
+      <c r="G25">
+        <v>8.7434999999999999E-2</v>
+      </c>
+      <c r="H25">
+        <v>0.57406400000000002</v>
+      </c>
+      <c r="I25">
+        <v>15</v>
+      </c>
+      <c r="J25">
+        <v>20</v>
+      </c>
+      <c r="K25">
+        <v>1.4652E-2</v>
+      </c>
+      <c r="L25">
+        <v>2.5585199999999999E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="M26">
+        <f>(M21+M23+M24)/3</f>
+        <v>713.44015329810657</v>
+      </c>
+      <c r="N26">
+        <f>(N21+N23+N24)/3</f>
+        <v>80.935199129672654</v>
+      </c>
+      <c r="O26">
+        <f>(O21+O23+O24)/3</f>
+        <v>107.94519108777611</v>
       </c>
     </row>
   </sheetData>
@@ -22680,21 +23405,21 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:AO12"/>
+  <dimension ref="A3:AO39"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="AO1" sqref="AO1:AO1048576"/>
+    <sheetView showRuler="0" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.1640625" customWidth="1"/>
-    <col min="5" max="5" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="2.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="2.6640625" bestFit="1" customWidth="1"/>
@@ -22704,7 +23429,7 @@
     <col min="14" max="14" width="2.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.83203125" style="18" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.1640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.6640625" style="18" customWidth="1"/>
     <col min="18" max="18" width="2.6640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="2.6640625" bestFit="1" customWidth="1"/>
@@ -22736,13 +23461,13 @@
       <c r="O3" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="U3" t="s">
+      <c r="S3" t="s">
         <v>57</v>
       </c>
+      <c r="Y3" t="s">
+        <v>65</v>
+      </c>
       <c r="AC3" t="s">
-        <v>65</v>
-      </c>
-      <c r="AK3" t="s">
         <v>64</v>
       </c>
     </row>
@@ -22771,1044 +23496,2167 @@
       <c r="O4" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="Q4" s="18" t="s">
-        <v>49</v>
+      <c r="Q4" t="s">
+        <v>47</v>
       </c>
       <c r="S4" t="s">
+        <v>62</v>
+      </c>
+      <c r="U4" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="W4" t="s">
         <v>47</v>
       </c>
-      <c r="U4" t="s">
+      <c r="Y4" t="s">
         <v>62</v>
       </c>
-      <c r="W4" s="18" t="s">
+      <c r="AA4" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="Y4" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA4" t="s">
+      <c r="AC4" t="s">
         <v>47</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AE4" t="s">
         <v>62</v>
       </c>
-      <c r="AE4" s="18" t="s">
+      <c r="AG4" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="AG4" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>47</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM4" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="AO4" s="18" t="s">
-        <v>49</v>
-      </c>
+      <c r="AM4"/>
+      <c r="AO4"/>
     </row>
     <row r="5" spans="1:41">
       <c r="A5">
         <v>1000</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C5">
         <v>0.1</v>
       </c>
       <c r="D5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E5">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G5" s="15">
         <v>0.1</v>
       </c>
       <c r="H5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I5">
         <v>34</v>
       </c>
       <c r="J5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K5">
         <v>37</v>
       </c>
       <c r="L5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M5">
         <v>55</v>
       </c>
       <c r="N5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O5" s="18">
         <v>0.84220700000000004</v>
       </c>
       <c r="P5" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q5" s="18">
-        <v>0.91300000000000003</v>
-      </c>
-      <c r="R5" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="Q5">
+        <v>60</v>
+      </c>
+      <c r="R5" s="16" t="s">
+        <v>71</v>
       </c>
       <c r="S5">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="T5" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="U5">
-        <v>64</v>
+        <v>71</v>
+      </c>
+      <c r="U5" s="18">
+        <v>0.75763000000000003</v>
       </c>
       <c r="V5" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="W5" s="18">
-        <v>0.75763000000000003</v>
+        <v>71</v>
+      </c>
+      <c r="W5">
+        <v>49</v>
       </c>
       <c r="X5" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y5" s="18">
-        <v>3.1135099999999999E-2</v>
+        <v>71</v>
+      </c>
+      <c r="Y5">
+        <v>76</v>
       </c>
       <c r="Z5" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA5">
-        <v>49</v>
+        <v>71</v>
+      </c>
+      <c r="AA5" s="18">
+        <v>0.824627</v>
       </c>
       <c r="AB5" s="16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AC5">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="AD5" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AE5" s="18">
-        <v>0.824627</v>
+        <v>71</v>
+      </c>
+      <c r="AE5">
+        <v>59</v>
       </c>
       <c r="AF5" s="16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AG5" s="18">
-        <v>0.25547599999999998</v>
-      </c>
-      <c r="AH5" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AI5">
-        <v>40</v>
-      </c>
-      <c r="AJ5" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AK5">
-        <v>59</v>
-      </c>
-      <c r="AL5" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AM5" s="18">
         <v>0.83953800000000001</v>
       </c>
-      <c r="AN5" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AO5" s="18">
-        <v>0.91206200000000004</v>
-      </c>
+      <c r="AH5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AM5"/>
+      <c r="AO5"/>
     </row>
     <row r="6" spans="1:41">
       <c r="A6">
         <v>1000</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C6">
         <v>0.1</v>
       </c>
       <c r="D6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E6">
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G6" s="15">
         <v>0.5</v>
       </c>
       <c r="H6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I6">
         <v>44</v>
       </c>
       <c r="J6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K6">
         <v>62</v>
       </c>
       <c r="L6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M6">
         <v>153</v>
       </c>
       <c r="N6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O6" s="18">
         <v>0.40223599999999998</v>
       </c>
       <c r="P6" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q6" s="18">
-        <v>0.85499999999999998</v>
-      </c>
-      <c r="R6" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="Q6">
+        <v>87</v>
+      </c>
+      <c r="R6" s="16" t="s">
+        <v>71</v>
       </c>
       <c r="S6">
-        <v>87</v>
+        <v>116</v>
       </c>
       <c r="T6" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="U6">
-        <v>116</v>
+        <v>71</v>
+      </c>
+      <c r="U6" s="18">
+        <v>0.280053</v>
       </c>
       <c r="V6" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="W6" s="18">
-        <v>0.280053</v>
+        <v>71</v>
+      </c>
+      <c r="W6">
+        <v>83</v>
       </c>
       <c r="X6" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y6" s="18">
-        <v>1.5886999999999998E-2</v>
+        <v>71</v>
+      </c>
+      <c r="Y6">
+        <v>158</v>
       </c>
       <c r="Z6" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA6">
-        <v>83</v>
+        <v>71</v>
+      </c>
+      <c r="AA6" s="18">
+        <v>0.36341600000000002</v>
       </c>
       <c r="AB6" s="16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AC6">
+        <v>68</v>
+      </c>
+      <c r="AD6" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE6">
         <v>158</v>
       </c>
-      <c r="AD6" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AE6" s="18">
-        <v>0.36341600000000002</v>
-      </c>
       <c r="AF6" s="16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AG6" s="18">
-        <v>8.9420100000000002E-2</v>
-      </c>
-      <c r="AH6" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AI6">
-        <v>68</v>
-      </c>
-      <c r="AJ6" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AK6">
-        <v>158</v>
-      </c>
-      <c r="AL6" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AM6" s="18">
         <v>0.39464700000000003</v>
       </c>
-      <c r="AN6" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AO6" s="18">
-        <v>0.25410100000000002</v>
-      </c>
+      <c r="AH6" t="s">
+        <v>72</v>
+      </c>
+      <c r="AM6"/>
+      <c r="AO6"/>
     </row>
     <row r="7" spans="1:41">
       <c r="A7" s="16">
         <v>1000</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C7" s="16">
         <v>0.1</v>
       </c>
       <c r="D7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E7" s="16">
         <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G7" s="17">
         <v>0.1</v>
       </c>
       <c r="H7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I7" s="16">
         <v>51</v>
       </c>
       <c r="J7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K7" s="16">
         <v>58</v>
       </c>
       <c r="L7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M7" s="16">
         <v>30</v>
       </c>
       <c r="N7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O7" s="18">
         <v>-1.98088E-3</v>
       </c>
       <c r="P7" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q7" s="18">
-        <v>0.73199999999999998</v>
-      </c>
-      <c r="R7" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="Q7">
+        <v>76</v>
+      </c>
+      <c r="R7" s="16" t="s">
+        <v>71</v>
       </c>
       <c r="S7">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="T7" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="U7">
-        <v>46</v>
+        <v>71</v>
+      </c>
+      <c r="U7" s="18">
+        <v>-1.8992200000000001E-3</v>
       </c>
       <c r="V7" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="W7" s="18">
-        <v>-1.8992200000000001E-3</v>
+        <v>71</v>
+      </c>
+      <c r="W7">
+        <v>65</v>
       </c>
       <c r="X7" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y7" s="18">
-        <v>2.4927899999999999E-2</v>
+        <v>71</v>
+      </c>
+      <c r="Y7">
+        <v>39</v>
       </c>
       <c r="Z7" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA7">
-        <v>65</v>
+        <v>71</v>
+      </c>
+      <c r="AA7" s="18">
+        <v>-1.9928599999999999E-3</v>
       </c>
       <c r="AB7" s="16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AC7">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="AD7" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AE7" s="18">
-        <v>-1.9928599999999999E-3</v>
+        <v>71</v>
+      </c>
+      <c r="AE7">
+        <v>35</v>
       </c>
       <c r="AF7" s="16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AG7" s="18">
-        <v>0.159332</v>
-      </c>
-      <c r="AH7" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AI7">
-        <v>61</v>
-      </c>
-      <c r="AJ7" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AK7">
-        <v>35</v>
-      </c>
-      <c r="AL7" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AM7" s="18">
         <v>-2.2480199999999999E-3</v>
       </c>
-      <c r="AN7" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AO7" s="18">
-        <v>0.54999600000000004</v>
-      </c>
+      <c r="AH7" t="s">
+        <v>72</v>
+      </c>
+      <c r="AM7"/>
+      <c r="AO7"/>
     </row>
     <row r="8" spans="1:41">
       <c r="A8" s="16">
         <v>1000</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C8" s="16">
         <v>0.1</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E8" s="16">
         <v>8</v>
       </c>
       <c r="F8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G8" s="15">
         <v>0.5</v>
       </c>
       <c r="H8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I8" s="16">
         <v>130</v>
       </c>
       <c r="J8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K8" s="16">
         <v>74</v>
       </c>
       <c r="L8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M8" s="16">
         <v>68</v>
       </c>
       <c r="N8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O8" s="18">
         <v>3.02247E-2</v>
       </c>
       <c r="P8" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q8" s="18">
-        <v>0.35799999999999998</v>
-      </c>
-      <c r="R8" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="Q8">
+        <v>74</v>
+      </c>
+      <c r="R8" s="16" t="s">
+        <v>71</v>
       </c>
       <c r="S8">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="T8" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="U8">
-        <v>56</v>
+        <v>71</v>
+      </c>
+      <c r="U8" s="18">
+        <v>1.9789500000000002E-2</v>
       </c>
       <c r="V8" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="W8" s="18">
-        <v>1.9789500000000002E-2</v>
+        <v>71</v>
+      </c>
+      <c r="W8">
+        <v>79</v>
       </c>
       <c r="X8" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y8" s="18">
-        <v>5.0818900000000004E-3</v>
+        <v>71</v>
+      </c>
+      <c r="Y8">
+        <v>66</v>
       </c>
       <c r="Z8" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA8">
+        <v>71</v>
+      </c>
+      <c r="AA8" s="18">
+        <v>2.77805E-2</v>
+      </c>
+      <c r="AB8" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC8">
         <v>79</v>
       </c>
-      <c r="AB8" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AC8">
-        <v>66</v>
-      </c>
       <c r="AD8" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AE8" s="18">
-        <v>2.77805E-2</v>
+        <v>71</v>
+      </c>
+      <c r="AE8">
+        <v>72</v>
       </c>
       <c r="AF8" s="16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AG8" s="18">
-        <v>1.5967100000000001E-2</v>
-      </c>
-      <c r="AH8" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AI8">
-        <v>79</v>
-      </c>
-      <c r="AJ8" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AK8">
+        <v>3.0200299999999999E-2</v>
+      </c>
+      <c r="AH8" t="s">
         <v>72</v>
       </c>
-      <c r="AL8" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AM8" s="18">
-        <v>3.0200299999999999E-2</v>
-      </c>
-      <c r="AN8" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AO8" s="18">
-        <v>4.1770000000000002E-2</v>
-      </c>
+      <c r="AM8"/>
+      <c r="AO8"/>
     </row>
     <row r="9" spans="1:41">
       <c r="A9" s="16">
         <v>1000</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C9" s="16">
         <v>0.3</v>
       </c>
       <c r="D9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E9" s="16">
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G9" s="17">
         <v>0.1</v>
       </c>
       <c r="H9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I9" s="16">
         <v>35</v>
       </c>
       <c r="J9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K9" s="16">
         <v>50</v>
       </c>
       <c r="L9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M9" s="16">
         <v>53</v>
       </c>
       <c r="N9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O9" s="18">
         <v>0.61209499999999994</v>
       </c>
       <c r="P9" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q9" s="18">
-        <v>0.59199999999999997</v>
-      </c>
-      <c r="R9" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="Q9">
+        <v>69</v>
+      </c>
+      <c r="R9" s="16" t="s">
+        <v>71</v>
       </c>
       <c r="S9">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T9" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="U9">
-        <v>67</v>
+        <v>71</v>
+      </c>
+      <c r="U9" s="18">
+        <v>0.46099600000000002</v>
       </c>
       <c r="V9" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="W9" s="18">
-        <v>0.46099600000000002</v>
+        <v>71</v>
+      </c>
+      <c r="W9">
+        <v>64</v>
       </c>
       <c r="X9" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y9" s="18">
-        <v>1.3454000000000001E-2</v>
+        <v>71</v>
+      </c>
+      <c r="Y9">
+        <v>73</v>
       </c>
       <c r="Z9" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA9">
-        <v>64</v>
+        <v>71</v>
+      </c>
+      <c r="AA9" s="18">
+        <v>0.57736399999999999</v>
       </c>
       <c r="AB9" s="16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AC9">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="AD9" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AE9" s="18">
-        <v>0.57736399999999999</v>
+        <v>71</v>
+      </c>
+      <c r="AE9">
+        <v>60</v>
       </c>
       <c r="AF9" s="16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AG9" s="18">
-        <v>9.0029999999999999E-2</v>
-      </c>
-      <c r="AH9" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AI9">
-        <v>55</v>
-      </c>
-      <c r="AJ9" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AK9">
-        <v>60</v>
-      </c>
-      <c r="AL9" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AM9" s="18">
         <v>0.60531000000000001</v>
       </c>
-      <c r="AN9" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AO9" s="18">
-        <v>0.32089499999999999</v>
-      </c>
+      <c r="AH9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AM9"/>
+      <c r="AO9"/>
     </row>
     <row r="10" spans="1:41">
       <c r="A10" s="16">
         <v>1000</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C10" s="16">
         <v>0.3</v>
       </c>
       <c r="D10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E10" s="16">
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G10" s="15">
         <v>0.5</v>
       </c>
       <c r="H10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I10" s="16">
         <v>44</v>
       </c>
       <c r="J10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K10" s="16">
         <v>60</v>
       </c>
       <c r="L10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M10" s="16">
         <v>95</v>
       </c>
       <c r="N10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O10" s="18">
         <v>0.19318299999999999</v>
       </c>
       <c r="P10" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q10" s="18">
-        <v>0.434</v>
-      </c>
-      <c r="R10" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="Q10">
+        <v>92</v>
+      </c>
+      <c r="R10" s="16" t="s">
+        <v>71</v>
       </c>
       <c r="S10">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="T10" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="U10">
-        <v>93</v>
+        <v>71</v>
+      </c>
+      <c r="U10" s="18">
+        <v>0.109227</v>
       </c>
       <c r="V10" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="W10" s="18">
-        <v>0.109227</v>
+        <v>71</v>
+      </c>
+      <c r="W10">
+        <v>85</v>
       </c>
       <c r="X10" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y10" s="18">
-        <v>6.2849500000000001E-3</v>
+        <v>71</v>
+      </c>
+      <c r="Y10">
+        <v>102</v>
       </c>
       <c r="Z10" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA10">
-        <v>85</v>
+        <v>71</v>
+      </c>
+      <c r="AA10" s="18">
+        <v>0.15245600000000001</v>
       </c>
       <c r="AB10" s="16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AC10">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="AD10" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AE10" s="18">
-        <v>0.15245600000000001</v>
+        <v>71</v>
+      </c>
+      <c r="AE10">
+        <v>106</v>
       </c>
       <c r="AF10" s="16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AG10" s="18">
-        <v>2.3877900000000001E-2</v>
-      </c>
-      <c r="AH10" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AI10">
-        <v>77</v>
-      </c>
-      <c r="AJ10" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AK10">
-        <v>106</v>
-      </c>
-      <c r="AL10" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AM10" s="18">
         <v>0.16934299999999999</v>
       </c>
-      <c r="AN10" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AO10" s="18">
-        <v>6.83589E-2</v>
-      </c>
+      <c r="AH10" t="s">
+        <v>72</v>
+      </c>
+      <c r="AM10"/>
+      <c r="AO10"/>
     </row>
     <row r="11" spans="1:41">
       <c r="A11" s="16">
         <v>1000</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C11" s="16">
         <v>0.3</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E11" s="16">
         <v>8</v>
       </c>
       <c r="F11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G11" s="17">
         <v>0.1</v>
       </c>
       <c r="H11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I11" s="16">
         <v>48</v>
       </c>
       <c r="J11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K11" s="16">
         <v>64</v>
       </c>
       <c r="L11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M11" s="16">
         <v>35</v>
       </c>
       <c r="N11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O11" s="18">
         <v>0.30381599999999997</v>
       </c>
       <c r="P11" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q11" s="18">
-        <v>0.47199999999999998</v>
-      </c>
-      <c r="R11" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="Q11">
+        <v>79</v>
+      </c>
+      <c r="R11" s="16" t="s">
+        <v>71</v>
       </c>
       <c r="S11">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="T11" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="U11">
-        <v>59</v>
+        <v>71</v>
+      </c>
+      <c r="U11" s="18">
+        <v>0.23926600000000001</v>
       </c>
       <c r="V11" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="W11" s="18">
-        <v>0.23926600000000001</v>
+        <v>71</v>
+      </c>
+      <c r="W11">
+        <v>74</v>
       </c>
       <c r="X11" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y11" s="18">
-        <v>1.1403099999999999E-2</v>
+        <v>71</v>
+      </c>
+      <c r="Y11">
+        <v>55</v>
       </c>
       <c r="Z11" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA11">
-        <v>74</v>
+        <v>71</v>
+      </c>
+      <c r="AA11" s="18">
+        <v>0.292717</v>
       </c>
       <c r="AB11" s="16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AC11">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="AD11" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AE11" s="18">
-        <v>0.292717</v>
+        <v>71</v>
+      </c>
+      <c r="AE11">
+        <v>46</v>
       </c>
       <c r="AF11" s="16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AG11" s="18">
-        <v>6.3992999999999994E-2</v>
-      </c>
-      <c r="AH11" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AI11">
-        <v>69</v>
-      </c>
-      <c r="AJ11" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AK11">
-        <v>46</v>
-      </c>
-      <c r="AL11" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AM11" s="18">
         <v>0.30113499999999999</v>
       </c>
-      <c r="AN11" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AO11" s="18">
-        <v>0.20505200000000001</v>
-      </c>
+      <c r="AH11" t="s">
+        <v>72</v>
+      </c>
+      <c r="AM11"/>
+      <c r="AO11"/>
     </row>
     <row r="12" spans="1:41">
       <c r="A12" s="16">
         <v>1000</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C12" s="16">
         <v>0.3</v>
       </c>
       <c r="D12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E12" s="16">
         <v>8</v>
       </c>
       <c r="F12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G12" s="15">
         <v>0.5</v>
       </c>
       <c r="H12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I12" s="16">
         <v>142</v>
       </c>
       <c r="J12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K12" s="16">
         <v>57</v>
       </c>
       <c r="L12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M12" s="16">
         <v>43</v>
       </c>
       <c r="N12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O12" s="18">
         <v>1.8854200000000002E-2</v>
       </c>
       <c r="P12" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q12" s="18">
+        <v>71</v>
+      </c>
+      <c r="Q12">
+        <v>58</v>
+      </c>
+      <c r="R12" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="S12">
+        <v>46</v>
+      </c>
+      <c r="T12" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="U12" s="18">
+        <v>1.28416E-2</v>
+      </c>
+      <c r="V12" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="W12">
+        <v>61</v>
+      </c>
+      <c r="X12" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y12">
+        <v>49</v>
+      </c>
+      <c r="Z12" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA12" s="18">
+        <v>1.6754499999999999E-2</v>
+      </c>
+      <c r="AB12" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC12">
+        <v>59</v>
+      </c>
+      <c r="AD12" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE12">
+        <v>45</v>
+      </c>
+      <c r="AF12" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG12" s="18">
+        <v>1.7733599999999999E-2</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>72</v>
+      </c>
+      <c r="AM12"/>
+      <c r="AO12"/>
+    </row>
+    <row r="18" spans="1:41">
+      <c r="I18" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="M18" t="s">
+        <v>57</v>
+      </c>
+      <c r="S18" t="s">
+        <v>65</v>
+      </c>
+      <c r="T18" s="18"/>
+      <c r="V18" s="18"/>
+      <c r="W18"/>
+      <c r="Y18" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD18" s="18"/>
+      <c r="AE18"/>
+      <c r="AF18" s="18"/>
+      <c r="AG18"/>
+      <c r="AM18"/>
+      <c r="AO18"/>
+    </row>
+    <row r="19" spans="1:41">
+      <c r="A19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" t="s">
+        <v>54</v>
+      </c>
+      <c r="I19" t="s">
+        <v>74</v>
+      </c>
+      <c r="K19" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="M19" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="O19" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q19" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="S19" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="U19" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="W19" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y19" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE19"/>
+      <c r="AG19"/>
+      <c r="AM19"/>
+      <c r="AO19"/>
+    </row>
+    <row r="20" spans="1:41">
+      <c r="A20">
+        <v>1000</v>
+      </c>
+      <c r="B20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20">
+        <v>0.1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20" t="s">
+        <v>71</v>
+      </c>
+      <c r="G20" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="H20" t="s">
+        <v>71</v>
+      </c>
+      <c r="I20" s="18">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="J20" t="s">
+        <v>71</v>
+      </c>
+      <c r="K20" s="18">
+        <v>5.3818199999999998E-3</v>
+      </c>
+      <c r="L20" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="M20" s="18">
+        <v>3.1135099999999999E-2</v>
+      </c>
+      <c r="N20" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="O20" s="20">
+        <f>K20/M20*100</f>
+        <v>17.285378881069917</v>
+      </c>
+      <c r="P20" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q20" s="18">
+        <v>2.48542E-2</v>
+      </c>
+      <c r="R20" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="S20" s="18">
+        <v>0.25547599999999998</v>
+      </c>
+      <c r="T20" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="U20" s="20">
+        <f>Q20/S20*100</f>
+        <v>9.7285850725704179</v>
+      </c>
+      <c r="V20" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="W20" s="18">
+        <v>4.9728899999999999E-2</v>
+      </c>
+      <c r="X20" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y20" s="18">
+        <v>0.91206200000000004</v>
+      </c>
+      <c r="Z20" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA20" s="20">
+        <f>W20/Y20*100</f>
+        <v>5.4523595983606379</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE20">
+        <f>I20/W20*0.95</f>
+        <v>17.441568182686527</v>
+      </c>
+      <c r="AG20"/>
+      <c r="AM20"/>
+      <c r="AO20"/>
+    </row>
+    <row r="21" spans="1:41">
+      <c r="A21">
+        <v>1000</v>
+      </c>
+      <c r="B21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21">
+        <v>0.1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21" t="s">
+        <v>71</v>
+      </c>
+      <c r="G21" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="H21" t="s">
+        <v>71</v>
+      </c>
+      <c r="I21" s="18">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="J21" t="s">
+        <v>71</v>
+      </c>
+      <c r="K21" s="18">
+        <v>3.5009400000000001E-3</v>
+      </c>
+      <c r="L21" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="M21" s="18">
+        <v>1.5886999999999998E-2</v>
+      </c>
+      <c r="N21" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="O21" s="20">
+        <f>K21/M21*100</f>
+        <v>22.036507836595963</v>
+      </c>
+      <c r="P21" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q21" s="18">
+        <v>9.6750299999999994E-3</v>
+      </c>
+      <c r="R21" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="S21" s="18">
+        <v>8.9420100000000002E-2</v>
+      </c>
+      <c r="T21" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="U21" s="20">
+        <f>Q21/S21*100</f>
+        <v>10.819748580017244</v>
+      </c>
+      <c r="V21" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="W21" s="18">
+        <v>1.7358999999999999E-2</v>
+      </c>
+      <c r="X21" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y21" s="18">
+        <v>0.25410100000000002</v>
+      </c>
+      <c r="Z21" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA21" s="20">
+        <f>W21/Y21*100</f>
+        <v>6.831535491792633</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE21">
+        <f>I21/W21*0.95</f>
+        <v>46.791289820842216</v>
+      </c>
+      <c r="AG21"/>
+      <c r="AM21"/>
+      <c r="AO21"/>
+    </row>
+    <row r="22" spans="1:41">
+      <c r="A22" s="16">
+        <v>1000</v>
+      </c>
+      <c r="B22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="16">
+        <v>8</v>
+      </c>
+      <c r="F22" t="s">
+        <v>71</v>
+      </c>
+      <c r="G22" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="H22" t="s">
+        <v>71</v>
+      </c>
+      <c r="I22" s="18">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="J22" t="s">
+        <v>71</v>
+      </c>
+      <c r="K22" s="18">
+        <v>4.3480400000000001E-3</v>
+      </c>
+      <c r="L22" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="M22" s="18">
+        <v>2.4927899999999999E-2</v>
+      </c>
+      <c r="N22" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="O22" s="20">
+        <f>K22/M22*100</f>
+        <v>17.442464066367407</v>
+      </c>
+      <c r="P22" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q22" s="18">
+        <v>1.17419E-2</v>
+      </c>
+      <c r="R22" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="S22" s="18">
+        <v>0.159332</v>
+      </c>
+      <c r="T22" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="U22" s="20">
+        <f>Q22/S22*100</f>
+        <v>7.3694549745186144</v>
+      </c>
+      <c r="V22" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="W22" s="18">
+        <v>2.4364899999999998E-2</v>
+      </c>
+      <c r="X22" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y22" s="18">
+        <v>0.54999600000000004</v>
+      </c>
+      <c r="Z22" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA22" s="20">
+        <f>W22/Y22*100</f>
+        <v>4.4300140364657192</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE22">
+        <f t="shared" ref="AE22:AE27" si="0">I22/W22*0.95</f>
+        <v>28.541057012341525</v>
+      </c>
+      <c r="AG22"/>
+      <c r="AM22"/>
+      <c r="AO22"/>
+    </row>
+    <row r="23" spans="1:41">
+      <c r="A23" s="16">
+        <v>1000</v>
+      </c>
+      <c r="B23" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" s="16">
+        <v>8</v>
+      </c>
+      <c r="F23" t="s">
+        <v>71</v>
+      </c>
+      <c r="G23" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="H23" t="s">
+        <v>71</v>
+      </c>
+      <c r="I23" s="18">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="J23" t="s">
+        <v>71</v>
+      </c>
+      <c r="K23" s="18">
+        <v>2.1750900000000002E-3</v>
+      </c>
+      <c r="L23" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="M23" s="18">
+        <v>5.0818900000000004E-3</v>
+      </c>
+      <c r="N23" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="O23" s="20">
+        <f>K23/M23*100</f>
+        <v>42.80080836066896</v>
+      </c>
+      <c r="P23" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q23" s="18">
+        <v>5.7649600000000004E-3</v>
+      </c>
+      <c r="R23" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="S23" s="18">
+        <v>1.5967100000000001E-2</v>
+      </c>
+      <c r="T23" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="U23" s="20">
+        <f>Q23/S23*100</f>
+        <v>36.105241402634164</v>
+      </c>
+      <c r="V23" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="W23" s="18">
+        <v>1.1149900000000001E-2</v>
+      </c>
+      <c r="X23" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y23" s="18">
+        <v>4.1770000000000002E-2</v>
+      </c>
+      <c r="Z23" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA23" s="20">
+        <f>W23/Y23*100</f>
+        <v>26.693559971271245</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE23">
+        <f t="shared" si="0"/>
+        <v>30.502515717629752</v>
+      </c>
+      <c r="AG23"/>
+      <c r="AM23"/>
+      <c r="AO23"/>
+    </row>
+    <row r="24" spans="1:41">
+      <c r="A24" s="16">
+        <v>1000</v>
+      </c>
+      <c r="B24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="D24" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24" s="16">
+        <v>2</v>
+      </c>
+      <c r="F24" t="s">
+        <v>71</v>
+      </c>
+      <c r="G24" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="H24" t="s">
+        <v>71</v>
+      </c>
+      <c r="I24" s="18">
+        <v>0.59199999999999997</v>
+      </c>
+      <c r="J24" t="s">
+        <v>71</v>
+      </c>
+      <c r="K24" s="18">
+        <v>3.5028500000000001E-3</v>
+      </c>
+      <c r="L24" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="M24" s="18">
+        <v>1.3454000000000001E-2</v>
+      </c>
+      <c r="N24" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="O24" s="20">
+        <f>K24/M24*100</f>
+        <v>26.035751449383081</v>
+      </c>
+      <c r="P24" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q24" s="18">
+        <v>1.0603E-2</v>
+      </c>
+      <c r="R24" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="S24" s="18">
+        <v>9.0029999999999999E-2</v>
+      </c>
+      <c r="T24" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="U24" s="20">
+        <f>Q24/S24*100</f>
+        <v>11.777185382650227</v>
+      </c>
+      <c r="V24" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="W24" s="18">
+        <v>2.6727899999999999E-2</v>
+      </c>
+      <c r="X24" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y24" s="18">
+        <v>0.32089499999999999</v>
+      </c>
+      <c r="Z24" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA24" s="20">
+        <f>W24/Y24*100</f>
+        <v>8.3291730940027104</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE24">
+        <f t="shared" si="0"/>
+        <v>21.041683035330124</v>
+      </c>
+      <c r="AG24"/>
+      <c r="AM24"/>
+      <c r="AO24"/>
+    </row>
+    <row r="25" spans="1:41">
+      <c r="A25" s="16">
+        <v>1000</v>
+      </c>
+      <c r="B25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="D25" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" s="16">
+        <v>2</v>
+      </c>
+      <c r="F25" t="s">
+        <v>71</v>
+      </c>
+      <c r="G25" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="H25" t="s">
+        <v>71</v>
+      </c>
+      <c r="I25" s="18">
+        <v>0.434</v>
+      </c>
+      <c r="J25" t="s">
+        <v>71</v>
+      </c>
+      <c r="K25" s="18">
+        <v>2.3918199999999998E-3</v>
+      </c>
+      <c r="L25" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="M25" s="18">
+        <v>6.2849500000000001E-3</v>
+      </c>
+      <c r="N25" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="O25" s="20">
+        <f>K25/M25*100</f>
+        <v>38.056309119404283</v>
+      </c>
+      <c r="P25" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q25" s="18">
+        <v>6.4861800000000002E-3</v>
+      </c>
+      <c r="R25" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="S25" s="18">
+        <v>2.3877900000000001E-2</v>
+      </c>
+      <c r="T25" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="U25" s="20">
+        <f>Q25/S25*100</f>
+        <v>27.163946578216681</v>
+      </c>
+      <c r="V25" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="W25" s="18">
+        <v>1.25439E-2</v>
+      </c>
+      <c r="X25" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y25" s="18">
+        <v>6.83589E-2</v>
+      </c>
+      <c r="Z25" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA25" s="20">
+        <f>W25/Y25*100</f>
+        <v>18.350061220996828</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE25">
+        <f t="shared" si="0"/>
+        <v>32.868565597621149</v>
+      </c>
+      <c r="AG25"/>
+      <c r="AM25"/>
+      <c r="AO25"/>
+    </row>
+    <row r="26" spans="1:41">
+      <c r="A26" s="16">
+        <v>1000</v>
+      </c>
+      <c r="B26" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26" s="16">
+        <v>8</v>
+      </c>
+      <c r="F26" t="s">
+        <v>71</v>
+      </c>
+      <c r="G26" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="H26" t="s">
+        <v>71</v>
+      </c>
+      <c r="I26" s="18">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="J26" t="s">
+        <v>71</v>
+      </c>
+      <c r="K26" s="18">
+        <v>2.9330300000000001E-3</v>
+      </c>
+      <c r="L26" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="M26" s="18">
+        <v>1.1403099999999999E-2</v>
+      </c>
+      <c r="N26" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="O26" s="20">
+        <f>K26/M26*100</f>
+        <v>25.72133893414949</v>
+      </c>
+      <c r="P26" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q26" s="18">
+        <v>8.0151600000000003E-3</v>
+      </c>
+      <c r="R26" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="S26" s="18">
+        <v>6.3992999999999994E-2</v>
+      </c>
+      <c r="T26" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="U26" s="20">
+        <f>Q26/S26*100</f>
+        <v>12.525057428156206</v>
+      </c>
+      <c r="V26" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="W26" s="18">
+        <v>1.56069E-2</v>
+      </c>
+      <c r="X26" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y26" s="18">
+        <v>0.20505200000000001</v>
+      </c>
+      <c r="Z26" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA26" s="20">
+        <f>W26/Y26*100</f>
+        <v>7.6111913075707625</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE26">
+        <f t="shared" si="0"/>
+        <v>28.730881853539138</v>
+      </c>
+      <c r="AG26"/>
+      <c r="AM26"/>
+      <c r="AO26"/>
+    </row>
+    <row r="27" spans="1:41">
+      <c r="A27" s="16">
+        <v>1000</v>
+      </c>
+      <c r="B27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>71</v>
+      </c>
+      <c r="E27" s="16">
+        <v>8</v>
+      </c>
+      <c r="F27" t="s">
+        <v>71</v>
+      </c>
+      <c r="G27" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="H27" t="s">
+        <v>71</v>
+      </c>
+      <c r="I27" s="18">
         <v>0.32600000000000001</v>
       </c>
-      <c r="R12" t="s">
-        <v>70</v>
-      </c>
-      <c r="S12">
-        <v>58</v>
-      </c>
-      <c r="T12" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="U12">
+      <c r="J27" t="s">
+        <v>71</v>
+      </c>
+      <c r="K27" s="18">
+        <v>2.2480500000000001E-3</v>
+      </c>
+      <c r="L27" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="M27" s="18">
+        <v>4.5001499999999996E-3</v>
+      </c>
+      <c r="N27" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="O27" s="20">
+        <f>K27/M27*100</f>
+        <v>49.955001499950008</v>
+      </c>
+      <c r="P27" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q27" s="18">
+        <v>5.8739200000000004E-3</v>
+      </c>
+      <c r="R27" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="S27" s="18">
+        <v>1.0696900000000001E-2</v>
+      </c>
+      <c r="T27" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="U27" s="20">
+        <f>Q27/S27*100</f>
+        <v>54.912357785900589</v>
+      </c>
+      <c r="V27" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="W27" s="18">
+        <v>1.7472999999999999E-2</v>
+      </c>
+      <c r="X27" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y27" s="18">
+        <v>3.4079999999999999E-2</v>
+      </c>
+      <c r="Z27" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA27" s="20">
+        <f>W27/Y27*100</f>
+        <v>51.270539906103288</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE27">
+        <f t="shared" si="0"/>
+        <v>17.724489211926976</v>
+      </c>
+      <c r="AG27"/>
+      <c r="AM27"/>
+      <c r="AO27"/>
+    </row>
+    <row r="28" spans="1:41">
+      <c r="K28" s="18"/>
+      <c r="M28" s="18"/>
+      <c r="O28" s="18">
+        <f>SUM(O20:O27)/8</f>
+        <v>29.916695018448639</v>
+      </c>
+      <c r="S28" s="18"/>
+      <c r="U28" s="18">
+        <f>SUM(U20:U27)/8</f>
+        <v>21.300197150583017</v>
+      </c>
+      <c r="W28"/>
+      <c r="AA28" s="18">
+        <f>SUM(AA20:AA27)/8</f>
+        <v>16.121054328320479</v>
+      </c>
+      <c r="AE28">
+        <f>SUM(AE20:AE27)/8</f>
+        <v>27.955256303989671</v>
+      </c>
+      <c r="AI28" s="18"/>
+      <c r="AM28"/>
+      <c r="AO28"/>
+    </row>
+    <row r="33" spans="1:24">
+      <c r="G33" t="s">
+        <v>79</v>
+      </c>
+      <c r="L33" t="s">
+        <v>84</v>
+      </c>
+      <c r="R33" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24">
+      <c r="A34" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" t="s">
+        <v>47</v>
+      </c>
+      <c r="E34" t="s">
+        <v>80</v>
+      </c>
+      <c r="G34" t="s">
+        <v>81</v>
+      </c>
+      <c r="I34" t="s">
+        <v>47</v>
+      </c>
+      <c r="K34" t="s">
+        <v>80</v>
+      </c>
+      <c r="M34" t="s">
+        <v>82</v>
+      </c>
+      <c r="O34" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>47</v>
+      </c>
+      <c r="S34" t="s">
+        <v>80</v>
+      </c>
+      <c r="U34" t="s">
+        <v>82</v>
+      </c>
+      <c r="W34" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24">
+      <c r="A35" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35">
+        <v>4132</v>
+      </c>
+      <c r="D35" t="s">
+        <v>71</v>
+      </c>
+      <c r="E35">
+        <f>3228+1014+473+230+108+67+22+14+8+7+4+4+1</f>
+        <v>5180</v>
+      </c>
+      <c r="F35" t="s">
+        <v>71</v>
+      </c>
+      <c r="G35">
+        <v>68.459999999999994</v>
+      </c>
+      <c r="H35" t="s">
+        <v>71</v>
+      </c>
+      <c r="I35">
+        <v>3081</v>
+      </c>
+      <c r="J35" t="s">
+        <v>71</v>
+      </c>
+      <c r="K35">
+        <v>3937</v>
+      </c>
+      <c r="L35" t="s">
+        <v>71</v>
+      </c>
+      <c r="M35" s="18">
+        <v>0.13043299999999999</v>
+      </c>
+      <c r="N35" t="s">
+        <v>71</v>
+      </c>
+      <c r="O35" s="18">
+        <v>14.000299999999999</v>
+      </c>
+      <c r="P35" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q35">
+        <v>3070</v>
+      </c>
+      <c r="R35" t="s">
+        <v>71</v>
+      </c>
+      <c r="S35">
+        <v>4460</v>
+      </c>
+      <c r="T35" t="s">
+        <v>71</v>
+      </c>
+      <c r="U35" s="18">
+        <v>0.91746499999999997</v>
+      </c>
+      <c r="V35" t="s">
+        <v>71</v>
+      </c>
+      <c r="W35" s="18">
+        <v>417.15100000000001</v>
+      </c>
+      <c r="X35" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24">
+      <c r="A36" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" t="s">
+        <v>71</v>
+      </c>
+      <c r="E36" t="s">
+        <v>66</v>
+      </c>
+      <c r="F36" t="s">
+        <v>71</v>
+      </c>
+      <c r="G36" t="s">
+        <v>66</v>
+      </c>
+      <c r="H36" t="s">
+        <v>71</v>
+      </c>
+      <c r="I36">
+        <v>3947</v>
+      </c>
+      <c r="J36" t="s">
+        <v>71</v>
+      </c>
+      <c r="K36">
+        <v>4229</v>
+      </c>
+      <c r="L36" t="s">
+        <v>71</v>
+      </c>
+      <c r="M36" s="18">
+        <v>9.5930799999999997E-2</v>
+      </c>
+      <c r="N36" t="s">
+        <v>71</v>
+      </c>
+      <c r="O36" s="18">
+        <v>7.5047800000000002</v>
+      </c>
+      <c r="P36" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q36">
+        <v>2518</v>
+      </c>
+      <c r="R36" t="s">
+        <v>71</v>
+      </c>
+      <c r="S36">
+        <v>3899</v>
+      </c>
+      <c r="T36" t="s">
+        <v>71</v>
+      </c>
+      <c r="U36" s="18">
+        <v>0.81851499999999999</v>
+      </c>
+      <c r="V36" t="s">
+        <v>71</v>
+      </c>
+      <c r="W36" s="18">
+        <v>353.23599999999999</v>
+      </c>
+      <c r="X36" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24">
+      <c r="A37" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37">
+        <v>3675</v>
+      </c>
+      <c r="D37" t="s">
+        <v>71</v>
+      </c>
+      <c r="E37">
+        <f>2951+1096+228+29+4</f>
+        <v>4308</v>
+      </c>
+      <c r="F37" t="s">
+        <v>71</v>
+      </c>
+      <c r="G37">
+        <v>9.67</v>
+      </c>
+      <c r="H37" t="s">
+        <v>71</v>
+      </c>
+      <c r="I37">
+        <v>2185</v>
+      </c>
+      <c r="J37" t="s">
+        <v>71</v>
+      </c>
+      <c r="K37">
+        <v>1799</v>
+      </c>
+      <c r="L37" t="s">
+        <v>71</v>
+      </c>
+      <c r="M37" s="18">
+        <v>3.9567900000000003E-2</v>
+      </c>
+      <c r="N37" t="s">
+        <v>71</v>
+      </c>
+      <c r="O37" s="18">
+        <v>1.1317200000000001</v>
+      </c>
+      <c r="P37" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q37">
+        <v>3222</v>
+      </c>
+      <c r="R37" t="s">
+        <v>71</v>
+      </c>
+      <c r="S37">
+        <v>4154</v>
+      </c>
+      <c r="T37" t="s">
+        <v>71</v>
+      </c>
+      <c r="U37" s="18">
+        <v>0.300431</v>
+      </c>
+      <c r="V37" t="s">
+        <v>71</v>
+      </c>
+      <c r="W37" s="18">
+        <v>95.595799999999997</v>
+      </c>
+      <c r="X37" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24">
+      <c r="A38" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38">
+        <v>29</v>
+      </c>
+      <c r="D38" t="s">
+        <v>71</v>
+      </c>
+      <c r="E38">
+        <v>29</v>
+      </c>
+      <c r="F38" t="s">
+        <v>71</v>
+      </c>
+      <c r="G38">
+        <v>3.42</v>
+      </c>
+      <c r="H38" t="s">
+        <v>71</v>
+      </c>
+      <c r="I38">
+        <v>38</v>
+      </c>
+      <c r="J38" t="s">
+        <v>71</v>
+      </c>
+      <c r="K38">
         <v>46</v>
       </c>
-      <c r="V12" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="W12" s="18">
-        <v>1.28416E-2</v>
-      </c>
-      <c r="X12" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y12" s="18">
-        <v>4.5001499999999996E-3</v>
-      </c>
-      <c r="Z12" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA12">
-        <v>61</v>
-      </c>
-      <c r="AB12" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AC12">
-        <v>49</v>
-      </c>
-      <c r="AD12" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AE12" s="18">
-        <v>1.6754499999999999E-2</v>
-      </c>
-      <c r="AF12" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AG12" s="18">
-        <v>1.0696900000000001E-2</v>
-      </c>
-      <c r="AH12" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AI12">
-        <v>59</v>
-      </c>
-      <c r="AJ12" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AK12">
-        <v>45</v>
-      </c>
-      <c r="AL12" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AM12" s="18">
-        <v>1.7733599999999999E-2</v>
-      </c>
-      <c r="AN12" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AO12" s="18">
-        <v>3.4079999999999999E-2</v>
+      <c r="L38" t="s">
+        <v>71</v>
+      </c>
+      <c r="M38" s="21">
+        <v>2.30503E-3</v>
+      </c>
+      <c r="N38" t="s">
+        <v>71</v>
+      </c>
+      <c r="O38" s="18">
+        <v>1.1018E-2</v>
+      </c>
+      <c r="P38" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q38">
+        <v>19</v>
+      </c>
+      <c r="R38" t="s">
+        <v>71</v>
+      </c>
+      <c r="S38">
+        <v>27</v>
+      </c>
+      <c r="T38" t="s">
+        <v>71</v>
+      </c>
+      <c r="U38" s="18">
+        <v>2.29871E-2</v>
+      </c>
+      <c r="V38" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="W38" s="18">
+        <v>0.25202200000000002</v>
+      </c>
+      <c r="X38" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24">
+      <c r="A39" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" t="s">
+        <v>71</v>
+      </c>
+      <c r="C39" t="s">
+        <v>66</v>
+      </c>
+      <c r="D39" t="s">
+        <v>71</v>
+      </c>
+      <c r="E39" t="s">
+        <v>66</v>
+      </c>
+      <c r="F39" t="s">
+        <v>71</v>
+      </c>
+      <c r="G39" t="s">
+        <v>66</v>
+      </c>
+      <c r="H39" t="s">
+        <v>71</v>
+      </c>
+      <c r="I39">
+        <v>22</v>
+      </c>
+      <c r="J39" t="s">
+        <v>71</v>
+      </c>
+      <c r="K39">
+        <v>26</v>
+      </c>
+      <c r="L39" t="s">
+        <v>71</v>
+      </c>
+      <c r="M39" s="21">
+        <v>8.7434999999999999E-2</v>
+      </c>
+      <c r="N39" t="s">
+        <v>71</v>
+      </c>
+      <c r="O39" s="18">
+        <v>0.57406400000000002</v>
+      </c>
+      <c r="P39" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q39">
+        <v>15</v>
+      </c>
+      <c r="R39" t="s">
+        <v>71</v>
+      </c>
+      <c r="S39">
+        <v>20</v>
+      </c>
+      <c r="T39" t="s">
+        <v>71</v>
+      </c>
+      <c r="U39" s="18">
+        <v>1.4652E-2</v>
+      </c>
+      <c r="V39" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="W39" s="18">
+        <v>2.5585199999999999E-2</v>
+      </c>
+      <c r="X39" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>